<commit_message>
Update cleaning script - categories, depth, site
</commit_message>
<xml_diff>
--- a/R/2017_08_28_Completed_SemakauSeawall_Shallow (0m to 120m)_newcleaned.xlsx
+++ b/R/2017_08_28_Completed_SemakauSeawall_Shallow (0m to 120m)_newcleaned.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yeozy\Documents\Yale-NUS\Y3S1\UROPS\Data\R\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yeozy\Documents\Yale-NUS\Y3S1\UROPS\UROPS\R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{2740DA10-46A8-4053-B3D2-4A201E6762E2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{997441BB-4AC2-45EE-AC5F-7725F8FA9CA3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="521" yWindow="443" windowWidth="11609" windowHeight="15508" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,6 +17,9 @@
     <sheet name="Categories" sheetId="2" r:id="rId2"/>
     <sheet name="Semakau Seawall" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Semakau Seawall'!$A$1:$T$466</definedName>
+  </definedNames>
   <calcPr calcId="179017" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -9333,11 +9336,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:T465"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:T466"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A262" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F221" sqref="F221"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1796875" defaultRowHeight="16.100000000000001"/>
@@ -9372,7 +9376,7 @@
       <c r="G1" s="11" t="s">
         <v>894</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="32" t="s">
         <v>895</v>
       </c>
       <c r="I1" s="11" t="s">
@@ -9412,7 +9416,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:20" hidden="1">
       <c r="A2" s="20" t="s">
         <v>946</v>
       </c>
@@ -9444,7 +9448,7 @@
       <c r="J2" s="24"/>
       <c r="L2" s="43"/>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:20" hidden="1">
       <c r="A3" s="20" t="s">
         <v>946</v>
       </c>
@@ -9475,7 +9479,7 @@
       <c r="K3" s="43"/>
       <c r="L3" s="43"/>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:20" hidden="1">
       <c r="A4" s="20" t="s">
         <v>946</v>
       </c>
@@ -9506,7 +9510,7 @@
       <c r="K4" s="43"/>
       <c r="L4" s="43"/>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:20" hidden="1">
       <c r="A5" s="20" t="s">
         <v>946</v>
       </c>
@@ -9537,7 +9541,7 @@
       <c r="K5" s="43"/>
       <c r="L5" s="43"/>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:20" hidden="1">
       <c r="A6" s="20" t="s">
         <v>946</v>
       </c>
@@ -9568,7 +9572,7 @@
       <c r="K6" s="43"/>
       <c r="L6" s="43"/>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:20" hidden="1">
       <c r="A7" s="20" t="s">
         <v>946</v>
       </c>
@@ -9599,7 +9603,7 @@
       <c r="K7" s="43"/>
       <c r="L7" s="43"/>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:20" hidden="1">
       <c r="A8" s="20" t="s">
         <v>946</v>
       </c>
@@ -9630,7 +9634,7 @@
       <c r="K8" s="43"/>
       <c r="L8" s="43"/>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:20" hidden="1">
       <c r="A9" s="20" t="s">
         <v>946</v>
       </c>
@@ -9661,7 +9665,7 @@
       <c r="K9" s="43"/>
       <c r="L9" s="43"/>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:20" hidden="1">
       <c r="A10" s="20" t="s">
         <v>946</v>
       </c>
@@ -9692,7 +9696,7 @@
       <c r="K10" s="43"/>
       <c r="L10" s="43"/>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:20" hidden="1">
       <c r="A11" s="20" t="s">
         <v>946</v>
       </c>
@@ -9723,7 +9727,7 @@
       <c r="K11" s="43"/>
       <c r="L11" s="43"/>
     </row>
-    <row r="12" spans="1:20">
+    <row r="12" spans="1:20" hidden="1">
       <c r="A12" s="20" t="s">
         <v>946</v>
       </c>
@@ -9762,7 +9766,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="13" spans="1:20">
+    <row r="13" spans="1:20" hidden="1">
       <c r="A13" s="20" t="s">
         <v>946</v>
       </c>
@@ -9792,7 +9796,7 @@
       <c r="K13" s="43"/>
       <c r="L13" s="43"/>
     </row>
-    <row r="14" spans="1:20">
+    <row r="14" spans="1:20" hidden="1">
       <c r="A14" s="20" t="s">
         <v>946</v>
       </c>
@@ -9822,7 +9826,7 @@
       <c r="K14" s="43"/>
       <c r="L14" s="43"/>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15" spans="1:20" hidden="1">
       <c r="A15" s="20" t="s">
         <v>946</v>
       </c>
@@ -9852,7 +9856,7 @@
       <c r="K15" s="28"/>
       <c r="L15" s="43"/>
     </row>
-    <row r="16" spans="1:20">
+    <row r="16" spans="1:20" hidden="1">
       <c r="A16" s="20" t="s">
         <v>946</v>
       </c>
@@ -9882,7 +9886,7 @@
       <c r="K16" s="43"/>
       <c r="L16" s="43"/>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" hidden="1">
       <c r="A17" s="20" t="s">
         <v>946</v>
       </c>
@@ -9912,7 +9916,7 @@
       <c r="K17" s="28"/>
       <c r="L17" s="43"/>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" hidden="1">
       <c r="A18" s="20" t="s">
         <v>946</v>
       </c>
@@ -9942,7 +9946,7 @@
       <c r="K18" s="43"/>
       <c r="L18" s="43"/>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" hidden="1">
       <c r="A19" s="20" t="s">
         <v>946</v>
       </c>
@@ -9981,7 +9985,7 @@
         <v>971</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" hidden="1">
       <c r="A20" s="20" t="s">
         <v>946</v>
       </c>
@@ -10012,7 +10016,7 @@
       <c r="K20" s="43"/>
       <c r="L20" s="43"/>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:13" hidden="1">
       <c r="A21" s="20" t="s">
         <v>946</v>
       </c>
@@ -10044,7 +10048,7 @@
       <c r="J21" s="22"/>
       <c r="L21" s="43"/>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:13" hidden="1">
       <c r="A22" s="20" t="s">
         <v>946</v>
       </c>
@@ -10075,7 +10079,7 @@
       <c r="K22" s="43"/>
       <c r="L22" s="43"/>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:13" hidden="1">
       <c r="A23" s="20" t="s">
         <v>946</v>
       </c>
@@ -10114,7 +10118,7 @@
         <v>971</v>
       </c>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:13" hidden="1">
       <c r="A24" s="20" t="s">
         <v>946</v>
       </c>
@@ -10146,7 +10150,7 @@
       <c r="J24" s="22"/>
       <c r="L24" s="43"/>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:13" hidden="1">
       <c r="A25" s="20" t="s">
         <v>946</v>
       </c>
@@ -10176,7 +10180,7 @@
       <c r="J25" s="22"/>
       <c r="L25" s="43"/>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:13" hidden="1">
       <c r="A26" s="20" t="s">
         <v>946</v>
       </c>
@@ -10206,7 +10210,7 @@
       <c r="J26" s="22"/>
       <c r="L26" s="43"/>
     </row>
-    <row r="27" spans="1:13">
+    <row r="27" spans="1:13" hidden="1">
       <c r="A27" s="20" t="s">
         <v>946</v>
       </c>
@@ -10236,7 +10240,7 @@
       <c r="J27" s="22"/>
       <c r="L27" s="43"/>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" spans="1:13" hidden="1">
       <c r="A28" s="20" t="s">
         <v>946</v>
       </c>
@@ -10266,7 +10270,7 @@
       <c r="J28" s="22"/>
       <c r="L28" s="43"/>
     </row>
-    <row r="29" spans="1:13">
+    <row r="29" spans="1:13" hidden="1">
       <c r="A29" s="20" t="s">
         <v>946</v>
       </c>
@@ -10298,7 +10302,7 @@
       <c r="J29" s="22"/>
       <c r="L29" s="43"/>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:13" hidden="1">
       <c r="A30" s="20" t="s">
         <v>946</v>
       </c>
@@ -10329,7 +10333,7 @@
       <c r="K30" s="43"/>
       <c r="L30" s="43"/>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:13" hidden="1">
       <c r="A31" s="20" t="s">
         <v>946</v>
       </c>
@@ -10368,7 +10372,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" spans="1:13" hidden="1">
       <c r="A32" s="20" t="s">
         <v>946</v>
       </c>
@@ -10407,7 +10411,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="33" spans="1:13">
+    <row r="33" spans="1:13" hidden="1">
       <c r="A33" s="20" t="s">
         <v>946</v>
       </c>
@@ -10437,7 +10441,7 @@
       <c r="K33" s="43"/>
       <c r="L33" s="43"/>
     </row>
-    <row r="34" spans="1:13">
+    <row r="34" spans="1:13" hidden="1">
       <c r="A34" s="20" t="s">
         <v>946</v>
       </c>
@@ -10476,7 +10480,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="35" spans="1:13">
+    <row r="35" spans="1:13" hidden="1">
       <c r="A35" s="20" t="s">
         <v>946</v>
       </c>
@@ -10515,7 +10519,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="36" spans="1:13">
+    <row r="36" spans="1:13" hidden="1">
       <c r="A36" s="20" t="s">
         <v>946</v>
       </c>
@@ -10546,7 +10550,7 @@
       <c r="K36" s="43"/>
       <c r="L36" s="43"/>
     </row>
-    <row r="37" spans="1:13">
+    <row r="37" spans="1:13" hidden="1">
       <c r="A37" s="20" t="s">
         <v>946</v>
       </c>
@@ -10577,7 +10581,7 @@
       <c r="K37" s="43"/>
       <c r="L37" s="43"/>
     </row>
-    <row r="38" spans="1:13">
+    <row r="38" spans="1:13" hidden="1">
       <c r="A38" s="20" t="s">
         <v>946</v>
       </c>
@@ -10616,7 +10620,7 @@
         <v>1137</v>
       </c>
     </row>
-    <row r="39" spans="1:13">
+    <row r="39" spans="1:13" hidden="1">
       <c r="A39" s="20" t="s">
         <v>946</v>
       </c>
@@ -10647,7 +10651,7 @@
       <c r="K39" s="43"/>
       <c r="L39" s="43"/>
     </row>
-    <row r="40" spans="1:13">
+    <row r="40" spans="1:13" hidden="1">
       <c r="A40" s="20" t="s">
         <v>946</v>
       </c>
@@ -10678,7 +10682,7 @@
       <c r="K40" s="43"/>
       <c r="L40" s="43"/>
     </row>
-    <row r="41" spans="1:13">
+    <row r="41" spans="1:13" hidden="1">
       <c r="A41" s="20" t="s">
         <v>946</v>
       </c>
@@ -10709,7 +10713,7 @@
       <c r="K41" s="43"/>
       <c r="L41" s="43"/>
     </row>
-    <row r="42" spans="1:13">
+    <row r="42" spans="1:13" hidden="1">
       <c r="A42" s="20" t="s">
         <v>946</v>
       </c>
@@ -10740,7 +10744,7 @@
       <c r="K42" s="43"/>
       <c r="L42" s="43"/>
     </row>
-    <row r="43" spans="1:13">
+    <row r="43" spans="1:13" hidden="1">
       <c r="A43" s="20" t="s">
         <v>946</v>
       </c>
@@ -10771,7 +10775,7 @@
       <c r="K43" s="43"/>
       <c r="L43" s="43"/>
     </row>
-    <row r="44" spans="1:13">
+    <row r="44" spans="1:13" hidden="1">
       <c r="A44" s="20" t="s">
         <v>946</v>
       </c>
@@ -10802,7 +10806,7 @@
       <c r="K44" s="43"/>
       <c r="L44" s="43"/>
     </row>
-    <row r="45" spans="1:13">
+    <row r="45" spans="1:13" hidden="1">
       <c r="A45" s="20" t="s">
         <v>946</v>
       </c>
@@ -10842,7 +10846,7 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="46" spans="1:13">
+    <row r="46" spans="1:13" hidden="1">
       <c r="A46" s="20" t="s">
         <v>946</v>
       </c>
@@ -10873,7 +10877,7 @@
       <c r="K46" s="43"/>
       <c r="L46" s="43"/>
     </row>
-    <row r="47" spans="1:13">
+    <row r="47" spans="1:13" hidden="1">
       <c r="A47" s="20" t="s">
         <v>946</v>
       </c>
@@ -10913,7 +10917,7 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="48" spans="1:13">
+    <row r="48" spans="1:13" hidden="1">
       <c r="A48" s="20" t="s">
         <v>946</v>
       </c>
@@ -10953,7 +10957,7 @@
         <v>1119</v>
       </c>
     </row>
-    <row r="49" spans="1:13">
+    <row r="49" spans="1:13" hidden="1">
       <c r="A49" s="20" t="s">
         <v>946</v>
       </c>
@@ -10984,7 +10988,7 @@
       <c r="K49" s="43"/>
       <c r="L49" s="43"/>
     </row>
-    <row r="50" spans="1:13">
+    <row r="50" spans="1:13" hidden="1">
       <c r="A50" s="20" t="s">
         <v>946</v>
       </c>
@@ -11023,7 +11027,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="51" spans="1:13">
+    <row r="51" spans="1:13" hidden="1">
       <c r="A51" s="20" t="s">
         <v>946</v>
       </c>
@@ -11055,7 +11059,7 @@
       <c r="L51" s="43"/>
       <c r="M51" s="43"/>
     </row>
-    <row r="52" spans="1:13">
+    <row r="52" spans="1:13" hidden="1">
       <c r="A52" s="20" t="s">
         <v>946</v>
       </c>
@@ -11086,7 +11090,7 @@
       <c r="K52" s="43"/>
       <c r="L52" s="43"/>
     </row>
-    <row r="53" spans="1:13">
+    <row r="53" spans="1:13" hidden="1">
       <c r="A53" s="20" t="s">
         <v>946</v>
       </c>
@@ -11117,7 +11121,7 @@
       <c r="K53" s="43"/>
       <c r="L53" s="43"/>
     </row>
-    <row r="54" spans="1:13">
+    <row r="54" spans="1:13" hidden="1">
       <c r="A54" s="20" t="s">
         <v>946</v>
       </c>
@@ -11148,7 +11152,7 @@
       <c r="K54" s="43"/>
       <c r="L54" s="43"/>
     </row>
-    <row r="55" spans="1:13">
+    <row r="55" spans="1:13" hidden="1">
       <c r="A55" s="20" t="s">
         <v>946</v>
       </c>
@@ -11187,7 +11191,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="56" spans="1:13">
+    <row r="56" spans="1:13" hidden="1">
       <c r="A56" s="20" t="s">
         <v>946</v>
       </c>
@@ -11217,7 +11221,7 @@
       <c r="K56" s="43"/>
       <c r="L56" s="43"/>
     </row>
-    <row r="57" spans="1:13">
+    <row r="57" spans="1:13" hidden="1">
       <c r="A57" s="20" t="s">
         <v>946</v>
       </c>
@@ -11256,7 +11260,7 @@
         <v>1031</v>
       </c>
     </row>
-    <row r="58" spans="1:13">
+    <row r="58" spans="1:13" hidden="1">
       <c r="A58" s="20" t="s">
         <v>946</v>
       </c>
@@ -11295,7 +11299,7 @@
         <v>1120</v>
       </c>
     </row>
-    <row r="59" spans="1:13">
+    <row r="59" spans="1:13" hidden="1">
       <c r="A59" s="20" t="s">
         <v>946</v>
       </c>
@@ -11334,7 +11338,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="60" spans="1:13">
+    <row r="60" spans="1:13" hidden="1">
       <c r="A60" s="20" t="s">
         <v>946</v>
       </c>
@@ -11365,7 +11369,7 @@
       <c r="K60" s="43"/>
       <c r="L60" s="43"/>
     </row>
-    <row r="61" spans="1:13">
+    <row r="61" spans="1:13" hidden="1">
       <c r="A61" s="20" t="s">
         <v>946</v>
       </c>
@@ -11396,7 +11400,7 @@
       <c r="K61" s="43"/>
       <c r="L61" s="43"/>
     </row>
-    <row r="62" spans="1:13">
+    <row r="62" spans="1:13" hidden="1">
       <c r="A62" s="20" t="s">
         <v>946</v>
       </c>
@@ -11427,7 +11431,7 @@
       <c r="K62" s="43"/>
       <c r="L62" s="43"/>
     </row>
-    <row r="63" spans="1:13">
+    <row r="63" spans="1:13" hidden="1">
       <c r="A63" s="20" t="s">
         <v>946</v>
       </c>
@@ -11458,7 +11462,7 @@
       <c r="K63" s="43"/>
       <c r="L63" s="43"/>
     </row>
-    <row r="64" spans="1:13">
+    <row r="64" spans="1:13" hidden="1">
       <c r="A64" s="20" t="s">
         <v>946</v>
       </c>
@@ -11489,7 +11493,7 @@
       <c r="K64" s="43"/>
       <c r="L64" s="43"/>
     </row>
-    <row r="65" spans="1:13">
+    <row r="65" spans="1:13" hidden="1">
       <c r="A65" s="20" t="s">
         <v>946</v>
       </c>
@@ -11520,7 +11524,7 @@
       <c r="K65" s="43"/>
       <c r="L65" s="43"/>
     </row>
-    <row r="66" spans="1:13">
+    <row r="66" spans="1:13" hidden="1">
       <c r="A66" s="20" t="s">
         <v>946</v>
       </c>
@@ -11559,7 +11563,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="67" spans="1:13">
+    <row r="67" spans="1:13" hidden="1">
       <c r="A67" s="20" t="s">
         <v>946</v>
       </c>
@@ -11589,7 +11593,7 @@
       <c r="K67" s="43"/>
       <c r="L67" s="43"/>
     </row>
-    <row r="68" spans="1:13">
+    <row r="68" spans="1:13" hidden="1">
       <c r="A68" s="20" t="s">
         <v>946</v>
       </c>
@@ -11628,7 +11632,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="69" spans="1:13">
+    <row r="69" spans="1:13" hidden="1">
       <c r="A69" s="20" t="s">
         <v>946</v>
       </c>
@@ -11667,7 +11671,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="70" spans="1:13">
+    <row r="70" spans="1:13" hidden="1">
       <c r="A70" s="20" t="s">
         <v>946</v>
       </c>
@@ -11697,7 +11701,7 @@
       <c r="K70" s="28"/>
       <c r="L70" s="43"/>
     </row>
-    <row r="71" spans="1:13">
+    <row r="71" spans="1:13" hidden="1">
       <c r="A71" s="20" t="s">
         <v>946</v>
       </c>
@@ -11736,7 +11740,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="72" spans="1:13">
+    <row r="72" spans="1:13" hidden="1">
       <c r="A72" s="20" t="s">
         <v>946</v>
       </c>
@@ -11766,7 +11770,7 @@
       <c r="K72" s="43"/>
       <c r="L72" s="43"/>
     </row>
-    <row r="73" spans="1:13">
+    <row r="73" spans="1:13" hidden="1">
       <c r="A73" s="20" t="s">
         <v>946</v>
       </c>
@@ -11796,7 +11800,7 @@
       <c r="K73" s="43"/>
       <c r="L73" s="43"/>
     </row>
-    <row r="74" spans="1:13">
+    <row r="74" spans="1:13" hidden="1">
       <c r="A74" s="20" t="s">
         <v>946</v>
       </c>
@@ -11835,7 +11839,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="75" spans="1:13">
+    <row r="75" spans="1:13" hidden="1">
       <c r="A75" s="20" t="s">
         <v>946</v>
       </c>
@@ -11867,7 +11871,7 @@
         <v>1055</v>
       </c>
     </row>
-    <row r="76" spans="1:13">
+    <row r="76" spans="1:13" hidden="1">
       <c r="A76" s="20" t="s">
         <v>946</v>
       </c>
@@ -11906,7 +11910,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="77" spans="1:13">
+    <row r="77" spans="1:13" hidden="1">
       <c r="A77" s="20" t="s">
         <v>946</v>
       </c>
@@ -11936,7 +11940,7 @@
       <c r="K77" s="43"/>
       <c r="L77" s="43"/>
     </row>
-    <row r="78" spans="1:13">
+    <row r="78" spans="1:13" hidden="1">
       <c r="A78" s="20" t="s">
         <v>946</v>
       </c>
@@ -11975,7 +11979,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="79" spans="1:13">
+    <row r="79" spans="1:13" hidden="1">
       <c r="A79" s="20" t="s">
         <v>946</v>
       </c>
@@ -12011,7 +12015,7 @@
         <v>1121</v>
       </c>
     </row>
-    <row r="80" spans="1:13">
+    <row r="80" spans="1:13" hidden="1">
       <c r="A80" s="20" t="s">
         <v>946</v>
       </c>
@@ -12050,7 +12054,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="81" spans="1:13">
+    <row r="81" spans="1:13" hidden="1">
       <c r="A81" s="20" t="s">
         <v>946</v>
       </c>
@@ -12081,7 +12085,7 @@
       <c r="K81" s="43"/>
       <c r="L81" s="43"/>
     </row>
-    <row r="82" spans="1:13">
+    <row r="82" spans="1:13" hidden="1">
       <c r="A82" s="20" t="s">
         <v>946</v>
       </c>
@@ -12120,7 +12124,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="83" spans="1:13">
+    <row r="83" spans="1:13" hidden="1">
       <c r="A83" s="20" t="s">
         <v>946</v>
       </c>
@@ -12150,7 +12154,7 @@
       <c r="K83" s="43"/>
       <c r="L83" s="43"/>
     </row>
-    <row r="84" spans="1:13">
+    <row r="84" spans="1:13" hidden="1">
       <c r="A84" s="20" t="s">
         <v>946</v>
       </c>
@@ -12180,7 +12184,7 @@
       <c r="K84" s="28"/>
       <c r="L84" s="43"/>
     </row>
-    <row r="85" spans="1:13">
+    <row r="85" spans="1:13" hidden="1">
       <c r="A85" s="20" t="s">
         <v>946</v>
       </c>
@@ -12219,7 +12223,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="86" spans="1:13">
+    <row r="86" spans="1:13" hidden="1">
       <c r="A86" s="20" t="s">
         <v>946</v>
       </c>
@@ -12249,7 +12253,7 @@
       <c r="K86" s="28"/>
       <c r="L86" s="43"/>
     </row>
-    <row r="87" spans="1:13">
+    <row r="87" spans="1:13" hidden="1">
       <c r="A87" s="20" t="s">
         <v>946</v>
       </c>
@@ -12288,7 +12292,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="88" spans="1:13">
+    <row r="88" spans="1:13" hidden="1">
       <c r="A88" s="20" t="s">
         <v>946</v>
       </c>
@@ -12319,7 +12323,7 @@
       <c r="K88" s="43"/>
       <c r="L88" s="43"/>
     </row>
-    <row r="89" spans="1:13">
+    <row r="89" spans="1:13" hidden="1">
       <c r="A89" s="20" t="s">
         <v>946</v>
       </c>
@@ -12350,7 +12354,7 @@
       <c r="K89" s="43"/>
       <c r="L89" s="43"/>
     </row>
-    <row r="90" spans="1:13">
+    <row r="90" spans="1:13" hidden="1">
       <c r="A90" s="20" t="s">
         <v>946</v>
       </c>
@@ -12381,7 +12385,7 @@
       <c r="K90" s="43"/>
       <c r="L90" s="43"/>
     </row>
-    <row r="91" spans="1:13">
+    <row r="91" spans="1:13" hidden="1">
       <c r="A91" s="20" t="s">
         <v>946</v>
       </c>
@@ -12412,7 +12416,7 @@
       <c r="K91" s="43"/>
       <c r="L91" s="43"/>
     </row>
-    <row r="92" spans="1:13">
+    <row r="92" spans="1:13" hidden="1">
       <c r="A92" s="20" t="s">
         <v>946</v>
       </c>
@@ -12443,7 +12447,7 @@
       <c r="K92" s="43"/>
       <c r="L92" s="43"/>
     </row>
-    <row r="93" spans="1:13">
+    <row r="93" spans="1:13" hidden="1">
       <c r="A93" s="20" t="s">
         <v>946</v>
       </c>
@@ -12482,7 +12486,7 @@
         <v>1138</v>
       </c>
     </row>
-    <row r="94" spans="1:13">
+    <row r="94" spans="1:13" hidden="1">
       <c r="A94" s="20" t="s">
         <v>946</v>
       </c>
@@ -12513,7 +12517,7 @@
       <c r="K94" s="43"/>
       <c r="L94" s="43"/>
     </row>
-    <row r="95" spans="1:13">
+    <row r="95" spans="1:13" hidden="1">
       <c r="A95" s="20" t="s">
         <v>946</v>
       </c>
@@ -12544,7 +12548,7 @@
       <c r="K95" s="43"/>
       <c r="L95" s="43"/>
     </row>
-    <row r="96" spans="1:13">
+    <row r="96" spans="1:13" hidden="1">
       <c r="A96" s="20" t="s">
         <v>946</v>
       </c>
@@ -12575,7 +12579,7 @@
       <c r="K96" s="43"/>
       <c r="L96" s="43"/>
     </row>
-    <row r="97" spans="1:13">
+    <row r="97" spans="1:13" hidden="1">
       <c r="A97" s="20" t="s">
         <v>946</v>
       </c>
@@ -12614,7 +12618,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="98" spans="1:13">
+    <row r="98" spans="1:13" hidden="1">
       <c r="A98" s="20" t="s">
         <v>946</v>
       </c>
@@ -12645,7 +12649,7 @@
       <c r="K98" s="43"/>
       <c r="L98" s="43"/>
     </row>
-    <row r="99" spans="1:13">
+    <row r="99" spans="1:13" hidden="1">
       <c r="A99" s="20" t="s">
         <v>946</v>
       </c>
@@ -12676,7 +12680,7 @@
       <c r="K99" s="43"/>
       <c r="L99" s="43"/>
     </row>
-    <row r="100" spans="1:13">
+    <row r="100" spans="1:13" hidden="1">
       <c r="A100" s="20" t="s">
         <v>946</v>
       </c>
@@ -12707,7 +12711,7 @@
       <c r="K100" s="43"/>
       <c r="L100" s="43"/>
     </row>
-    <row r="101" spans="1:13">
+    <row r="101" spans="1:13" hidden="1">
       <c r="A101" s="20" t="s">
         <v>946</v>
       </c>
@@ -12746,7 +12750,7 @@
         <v>1031</v>
       </c>
     </row>
-    <row r="102" spans="1:13">
+    <row r="102" spans="1:13" hidden="1">
       <c r="A102" s="20" t="s">
         <v>946</v>
       </c>
@@ -12785,7 +12789,7 @@
         <v>1139</v>
       </c>
     </row>
-    <row r="103" spans="1:13">
+    <row r="103" spans="1:13" hidden="1">
       <c r="A103" s="20" t="s">
         <v>946</v>
       </c>
@@ -12815,7 +12819,7 @@
       <c r="K103" s="25"/>
       <c r="L103" s="43"/>
     </row>
-    <row r="104" spans="1:13">
+    <row r="104" spans="1:13" hidden="1">
       <c r="A104" s="20" t="s">
         <v>946</v>
       </c>
@@ -12845,7 +12849,7 @@
       <c r="K104" s="24"/>
       <c r="L104" s="43"/>
     </row>
-    <row r="105" spans="1:13">
+    <row r="105" spans="1:13" hidden="1">
       <c r="A105" s="20" t="s">
         <v>946</v>
       </c>
@@ -12875,7 +12879,7 @@
       <c r="K105" s="25"/>
       <c r="L105" s="43"/>
     </row>
-    <row r="106" spans="1:13">
+    <row r="106" spans="1:13" hidden="1">
       <c r="A106" s="20" t="s">
         <v>946</v>
       </c>
@@ -12914,7 +12918,7 @@
         <v>1031</v>
       </c>
     </row>
-    <row r="107" spans="1:13">
+    <row r="107" spans="1:13" hidden="1">
       <c r="A107" s="20" t="s">
         <v>946</v>
       </c>
@@ -12944,7 +12948,7 @@
       <c r="K107" s="24"/>
       <c r="L107" s="43"/>
     </row>
-    <row r="108" spans="1:13">
+    <row r="108" spans="1:13" hidden="1">
       <c r="A108" s="20" t="s">
         <v>946</v>
       </c>
@@ -12974,7 +12978,7 @@
       <c r="K108" s="25"/>
       <c r="L108" s="43"/>
     </row>
-    <row r="109" spans="1:13">
+    <row r="109" spans="1:13" hidden="1">
       <c r="A109" s="20" t="s">
         <v>946</v>
       </c>
@@ -13013,7 +13017,7 @@
         <v>1070</v>
       </c>
     </row>
-    <row r="110" spans="1:13">
+    <row r="110" spans="1:13" hidden="1">
       <c r="A110" s="20" t="s">
         <v>946</v>
       </c>
@@ -13043,7 +13047,7 @@
       <c r="K110" s="25"/>
       <c r="L110" s="43"/>
     </row>
-    <row r="111" spans="1:13">
+    <row r="111" spans="1:13" hidden="1">
       <c r="A111" s="20" t="s">
         <v>946</v>
       </c>
@@ -13082,7 +13086,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="112" spans="1:13">
+    <row r="112" spans="1:13" hidden="1">
       <c r="A112" s="20" t="s">
         <v>946</v>
       </c>
@@ -13112,7 +13116,7 @@
       <c r="K112" s="25"/>
       <c r="L112" s="43"/>
     </row>
-    <row r="113" spans="1:13">
+    <row r="113" spans="1:13" hidden="1">
       <c r="A113" s="20" t="s">
         <v>946</v>
       </c>
@@ -13151,7 +13155,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="114" spans="1:13">
+    <row r="114" spans="1:13" hidden="1">
       <c r="A114" s="20" t="s">
         <v>946</v>
       </c>
@@ -13182,7 +13186,7 @@
       <c r="K114" s="43"/>
       <c r="L114" s="43"/>
     </row>
-    <row r="115" spans="1:13">
+    <row r="115" spans="1:13" hidden="1">
       <c r="A115" s="20" t="s">
         <v>946</v>
       </c>
@@ -13214,7 +13218,7 @@
       <c r="J115" s="24"/>
       <c r="L115" s="43"/>
     </row>
-    <row r="116" spans="1:13">
+    <row r="116" spans="1:13" hidden="1">
       <c r="A116" s="20" t="s">
         <v>946</v>
       </c>
@@ -13244,7 +13248,7 @@
       <c r="J116" s="24"/>
       <c r="L116" s="43"/>
     </row>
-    <row r="117" spans="1:13">
+    <row r="117" spans="1:13" hidden="1">
       <c r="A117" s="20" t="s">
         <v>946</v>
       </c>
@@ -13276,7 +13280,7 @@
       <c r="J117" s="24"/>
       <c r="L117" s="43"/>
     </row>
-    <row r="118" spans="1:13">
+    <row r="118" spans="1:13" hidden="1">
       <c r="A118" s="20" t="s">
         <v>946</v>
       </c>
@@ -13302,7 +13306,7 @@
       <c r="K118" s="28"/>
       <c r="L118" s="28"/>
     </row>
-    <row r="119" spans="1:13">
+    <row r="119" spans="1:13" hidden="1">
       <c r="A119" s="19">
         <v>42975</v>
       </c>
@@ -13330,7 +13334,7 @@
       </c>
       <c r="K119" s="28"/>
     </row>
-    <row r="120" spans="1:13">
+    <row r="120" spans="1:13" hidden="1">
       <c r="A120" s="19">
         <v>42975</v>
       </c>
@@ -13358,7 +13362,7 @@
       </c>
       <c r="K120" s="28"/>
     </row>
-    <row r="121" spans="1:13">
+    <row r="121" spans="1:13" hidden="1">
       <c r="A121" s="19">
         <v>42975</v>
       </c>
@@ -13386,7 +13390,7 @@
       </c>
       <c r="K121" s="28"/>
     </row>
-    <row r="122" spans="1:13">
+    <row r="122" spans="1:13" hidden="1">
       <c r="A122" s="19">
         <v>42975</v>
       </c>
@@ -13425,7 +13429,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="123" spans="1:13">
+    <row r="123" spans="1:13" hidden="1">
       <c r="A123" s="19">
         <v>42975</v>
       </c>
@@ -13453,7 +13457,7 @@
       </c>
       <c r="K123" s="28"/>
     </row>
-    <row r="124" spans="1:13">
+    <row r="124" spans="1:13" hidden="1">
       <c r="A124" s="19">
         <v>42975</v>
       </c>
@@ -13481,7 +13485,7 @@
       </c>
       <c r="K124" s="28"/>
     </row>
-    <row r="125" spans="1:13">
+    <row r="125" spans="1:13" hidden="1">
       <c r="A125" s="19">
         <v>42975</v>
       </c>
@@ -13520,7 +13524,7 @@
         <v>1123</v>
       </c>
     </row>
-    <row r="126" spans="1:13">
+    <row r="126" spans="1:13" hidden="1">
       <c r="A126" s="19">
         <v>42975</v>
       </c>
@@ -13548,7 +13552,7 @@
       </c>
       <c r="K126" s="28"/>
     </row>
-    <row r="127" spans="1:13">
+    <row r="127" spans="1:13" hidden="1">
       <c r="A127" s="19">
         <v>42975</v>
       </c>
@@ -13576,7 +13580,7 @@
       </c>
       <c r="K127" s="28"/>
     </row>
-    <row r="128" spans="1:13">
+    <row r="128" spans="1:13" hidden="1">
       <c r="A128" s="19">
         <v>42975</v>
       </c>
@@ -13615,7 +13619,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="129" spans="1:13">
+    <row r="129" spans="1:13" hidden="1">
       <c r="A129" s="19">
         <v>42975</v>
       </c>
@@ -13643,7 +13647,7 @@
       </c>
       <c r="K129" s="28"/>
     </row>
-    <row r="130" spans="1:13">
+    <row r="130" spans="1:13" hidden="1">
       <c r="A130" s="19">
         <v>42975</v>
       </c>
@@ -13671,7 +13675,7 @@
       </c>
       <c r="K130" s="28"/>
     </row>
-    <row r="131" spans="1:13">
+    <row r="131" spans="1:13" hidden="1">
       <c r="A131" s="19">
         <v>42975</v>
       </c>
@@ -13710,7 +13714,7 @@
         <v>1120</v>
       </c>
     </row>
-    <row r="132" spans="1:13">
+    <row r="132" spans="1:13" hidden="1">
       <c r="A132" s="19">
         <v>42975</v>
       </c>
@@ -13738,7 +13742,7 @@
       </c>
       <c r="K132" s="28"/>
     </row>
-    <row r="133" spans="1:13">
+    <row r="133" spans="1:13" hidden="1">
       <c r="A133" s="19">
         <v>42975</v>
       </c>
@@ -13777,7 +13781,7 @@
         <v>1140</v>
       </c>
     </row>
-    <row r="134" spans="1:13">
+    <row r="134" spans="1:13" hidden="1">
       <c r="A134" s="19">
         <v>42975</v>
       </c>
@@ -13816,7 +13820,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="135" spans="1:13">
+    <row r="135" spans="1:13" hidden="1">
       <c r="A135" s="19">
         <v>42975</v>
       </c>
@@ -13844,7 +13848,7 @@
       </c>
       <c r="K135" s="28"/>
     </row>
-    <row r="136" spans="1:13">
+    <row r="136" spans="1:13" hidden="1">
       <c r="A136" s="19">
         <v>42975</v>
       </c>
@@ -13883,7 +13887,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="137" spans="1:13">
+    <row r="137" spans="1:13" hidden="1">
       <c r="A137" s="19">
         <v>42975</v>
       </c>
@@ -13911,7 +13915,7 @@
       </c>
       <c r="K137" s="28"/>
     </row>
-    <row r="138" spans="1:13">
+    <row r="138" spans="1:13" hidden="1">
       <c r="A138" s="19">
         <v>42975</v>
       </c>
@@ -13950,7 +13954,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="139" spans="1:13">
+    <row r="139" spans="1:13" hidden="1">
       <c r="A139" s="19">
         <v>42975</v>
       </c>
@@ -13978,7 +13982,7 @@
       </c>
       <c r="K139" s="28"/>
     </row>
-    <row r="140" spans="1:13">
+    <row r="140" spans="1:13" hidden="1">
       <c r="A140" s="19">
         <v>42975</v>
       </c>
@@ -14006,7 +14010,7 @@
       </c>
       <c r="K140" s="28"/>
     </row>
-    <row r="141" spans="1:13">
+    <row r="141" spans="1:13" hidden="1">
       <c r="A141" s="19">
         <v>42975</v>
       </c>
@@ -14034,7 +14038,7 @@
       </c>
       <c r="K141" s="28"/>
     </row>
-    <row r="142" spans="1:13">
+    <row r="142" spans="1:13" hidden="1">
       <c r="A142" s="19">
         <v>42975</v>
       </c>
@@ -14062,7 +14066,7 @@
       </c>
       <c r="K142" s="28"/>
     </row>
-    <row r="143" spans="1:13">
+    <row r="143" spans="1:13" hidden="1">
       <c r="A143" s="19">
         <v>42975</v>
       </c>
@@ -14101,7 +14105,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="144" spans="1:13">
+    <row r="144" spans="1:13" hidden="1">
       <c r="A144" s="19">
         <v>42975</v>
       </c>
@@ -14129,7 +14133,7 @@
       </c>
       <c r="K144" s="28"/>
     </row>
-    <row r="145" spans="1:13">
+    <row r="145" spans="1:13" hidden="1">
       <c r="A145" s="19">
         <v>42975</v>
       </c>
@@ -14157,7 +14161,7 @@
       </c>
       <c r="K145" s="28"/>
     </row>
-    <row r="146" spans="1:13">
+    <row r="146" spans="1:13" hidden="1">
       <c r="A146" s="19">
         <v>42975</v>
       </c>
@@ -14185,7 +14189,7 @@
       </c>
       <c r="K146" s="28"/>
     </row>
-    <row r="147" spans="1:13">
+    <row r="147" spans="1:13" hidden="1">
       <c r="A147" s="19">
         <v>42975</v>
       </c>
@@ -14213,7 +14217,7 @@
       </c>
       <c r="K147" s="28"/>
     </row>
-    <row r="148" spans="1:13">
+    <row r="148" spans="1:13" hidden="1">
       <c r="A148" s="19">
         <v>42975</v>
       </c>
@@ -14244,7 +14248,7 @@
       </c>
       <c r="K148" s="28"/>
     </row>
-    <row r="149" spans="1:13">
+    <row r="149" spans="1:13" hidden="1">
       <c r="A149" s="19">
         <v>42975</v>
       </c>
@@ -14272,7 +14276,7 @@
       </c>
       <c r="K149" s="28"/>
     </row>
-    <row r="150" spans="1:13">
+    <row r="150" spans="1:13" hidden="1">
       <c r="A150" s="19">
         <v>42975</v>
       </c>
@@ -14300,7 +14304,7 @@
       </c>
       <c r="K150" s="28"/>
     </row>
-    <row r="151" spans="1:13">
+    <row r="151" spans="1:13" hidden="1">
       <c r="A151" s="19">
         <v>42975</v>
       </c>
@@ -14328,7 +14332,7 @@
       </c>
       <c r="K151" s="28"/>
     </row>
-    <row r="152" spans="1:13">
+    <row r="152" spans="1:13" hidden="1">
       <c r="A152" s="19">
         <v>42975</v>
       </c>
@@ -14356,7 +14360,7 @@
       </c>
       <c r="K152" s="28"/>
     </row>
-    <row r="153" spans="1:13">
+    <row r="153" spans="1:13" hidden="1">
       <c r="A153" s="19">
         <v>42975</v>
       </c>
@@ -14384,7 +14388,7 @@
       </c>
       <c r="K153" s="28"/>
     </row>
-    <row r="154" spans="1:13">
+    <row r="154" spans="1:13" hidden="1">
       <c r="A154" s="19">
         <v>42975</v>
       </c>
@@ -14412,7 +14416,7 @@
       </c>
       <c r="K154" s="28"/>
     </row>
-    <row r="155" spans="1:13">
+    <row r="155" spans="1:13" hidden="1">
       <c r="A155" s="19">
         <v>42975</v>
       </c>
@@ -14440,7 +14444,7 @@
       </c>
       <c r="K155" s="28"/>
     </row>
-    <row r="156" spans="1:13">
+    <row r="156" spans="1:13" hidden="1">
       <c r="A156" s="19">
         <v>42975</v>
       </c>
@@ -14479,7 +14483,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="157" spans="1:13">
+    <row r="157" spans="1:13" hidden="1">
       <c r="A157" s="19">
         <v>42975</v>
       </c>
@@ -14507,7 +14511,7 @@
       </c>
       <c r="K157" s="28"/>
     </row>
-    <row r="158" spans="1:13">
+    <row r="158" spans="1:13" hidden="1">
       <c r="A158" s="19">
         <v>42975</v>
       </c>
@@ -14535,7 +14539,7 @@
       </c>
       <c r="K158" s="28"/>
     </row>
-    <row r="159" spans="1:13">
+    <row r="159" spans="1:13" hidden="1">
       <c r="A159" s="19">
         <v>42975</v>
       </c>
@@ -14563,7 +14567,7 @@
       </c>
       <c r="K159" s="28"/>
     </row>
-    <row r="160" spans="1:13">
+    <row r="160" spans="1:13" hidden="1">
       <c r="A160" s="19">
         <v>42975</v>
       </c>
@@ -14591,7 +14595,7 @@
       </c>
       <c r="K160" s="28"/>
     </row>
-    <row r="161" spans="1:13">
+    <row r="161" spans="1:13" hidden="1">
       <c r="A161" s="19">
         <v>42975</v>
       </c>
@@ -14619,7 +14623,7 @@
       </c>
       <c r="K161" s="28"/>
     </row>
-    <row r="162" spans="1:13">
+    <row r="162" spans="1:13" hidden="1">
       <c r="A162" s="19">
         <v>42975</v>
       </c>
@@ -14647,7 +14651,7 @@
       </c>
       <c r="K162" s="28"/>
     </row>
-    <row r="163" spans="1:13">
+    <row r="163" spans="1:13" hidden="1">
       <c r="A163" s="19">
         <v>42975</v>
       </c>
@@ -14678,7 +14682,7 @@
       </c>
       <c r="K163" s="28"/>
     </row>
-    <row r="164" spans="1:13">
+    <row r="164" spans="1:13" hidden="1">
       <c r="A164" s="19">
         <v>42975</v>
       </c>
@@ -14706,7 +14710,7 @@
       </c>
       <c r="K164" s="28"/>
     </row>
-    <row r="165" spans="1:13">
+    <row r="165" spans="1:13" hidden="1">
       <c r="A165" s="19">
         <v>42975</v>
       </c>
@@ -14734,7 +14738,7 @@
       </c>
       <c r="K165" s="28"/>
     </row>
-    <row r="166" spans="1:13">
+    <row r="166" spans="1:13" hidden="1">
       <c r="A166" s="19">
         <v>42975</v>
       </c>
@@ -14762,7 +14766,7 @@
       </c>
       <c r="K166" s="28"/>
     </row>
-    <row r="167" spans="1:13">
+    <row r="167" spans="1:13" hidden="1">
       <c r="A167" s="19">
         <v>42975</v>
       </c>
@@ -14790,7 +14794,7 @@
       </c>
       <c r="K167" s="28"/>
     </row>
-    <row r="168" spans="1:13">
+    <row r="168" spans="1:13" hidden="1">
       <c r="A168" s="19">
         <v>42975</v>
       </c>
@@ -14818,7 +14822,7 @@
       </c>
       <c r="K168" s="28"/>
     </row>
-    <row r="169" spans="1:13">
+    <row r="169" spans="1:13" hidden="1">
       <c r="A169" s="19">
         <v>42975</v>
       </c>
@@ -14846,7 +14850,7 @@
       </c>
       <c r="K169" s="28"/>
     </row>
-    <row r="170" spans="1:13">
+    <row r="170" spans="1:13" hidden="1">
       <c r="A170" s="19">
         <v>42975</v>
       </c>
@@ -14874,7 +14878,7 @@
       </c>
       <c r="K170" s="28"/>
     </row>
-    <row r="171" spans="1:13">
+    <row r="171" spans="1:13" hidden="1">
       <c r="A171" s="19">
         <v>42975</v>
       </c>
@@ -14902,7 +14906,7 @@
       </c>
       <c r="K171" s="28"/>
     </row>
-    <row r="172" spans="1:13">
+    <row r="172" spans="1:13" hidden="1">
       <c r="A172" s="19">
         <v>42975</v>
       </c>
@@ -14930,7 +14934,7 @@
       </c>
       <c r="K172" s="28"/>
     </row>
-    <row r="173" spans="1:13">
+    <row r="173" spans="1:13" hidden="1">
       <c r="A173" s="19">
         <v>42975</v>
       </c>
@@ -14961,7 +14965,7 @@
       </c>
       <c r="K173" s="28"/>
     </row>
-    <row r="174" spans="1:13">
+    <row r="174" spans="1:13" hidden="1">
       <c r="A174" s="19">
         <v>42975</v>
       </c>
@@ -15000,7 +15004,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="175" spans="1:13">
+    <row r="175" spans="1:13" hidden="1">
       <c r="A175" s="19">
         <v>42975</v>
       </c>
@@ -15028,7 +15032,7 @@
       </c>
       <c r="K175" s="28"/>
     </row>
-    <row r="176" spans="1:13">
+    <row r="176" spans="1:13" hidden="1">
       <c r="A176" s="19">
         <v>42975</v>
       </c>
@@ -15056,7 +15060,7 @@
       </c>
       <c r="K176" s="28"/>
     </row>
-    <row r="177" spans="1:13">
+    <row r="177" spans="1:13" hidden="1">
       <c r="A177" s="19">
         <v>42975</v>
       </c>
@@ -15084,7 +15088,7 @@
       </c>
       <c r="K177" s="28"/>
     </row>
-    <row r="178" spans="1:13">
+    <row r="178" spans="1:13" hidden="1">
       <c r="A178" s="19">
         <v>42975</v>
       </c>
@@ -15123,7 +15127,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="179" spans="1:13">
+    <row r="179" spans="1:13" hidden="1">
       <c r="A179" s="19">
         <v>42975</v>
       </c>
@@ -15151,7 +15155,7 @@
       </c>
       <c r="K179" s="28"/>
     </row>
-    <row r="180" spans="1:13">
+    <row r="180" spans="1:13" hidden="1">
       <c r="A180" s="19">
         <v>42975</v>
       </c>
@@ -15190,7 +15194,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="181" spans="1:13">
+    <row r="181" spans="1:13" hidden="1">
       <c r="A181" s="19">
         <v>42975</v>
       </c>
@@ -15218,7 +15222,7 @@
       </c>
       <c r="K181" s="28"/>
     </row>
-    <row r="182" spans="1:13">
+    <row r="182" spans="1:13" hidden="1">
       <c r="A182" s="19">
         <v>42975</v>
       </c>
@@ -15257,7 +15261,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="183" spans="1:13">
+    <row r="183" spans="1:13" hidden="1">
       <c r="A183" s="19">
         <v>42975</v>
       </c>
@@ -15285,7 +15289,7 @@
       </c>
       <c r="K183" s="28"/>
     </row>
-    <row r="184" spans="1:13">
+    <row r="184" spans="1:13" hidden="1">
       <c r="A184" s="19">
         <v>42975</v>
       </c>
@@ -15313,7 +15317,7 @@
       </c>
       <c r="K184" s="28"/>
     </row>
-    <row r="185" spans="1:13">
+    <row r="185" spans="1:13" hidden="1">
       <c r="A185" s="19">
         <v>42975</v>
       </c>
@@ -15341,7 +15345,7 @@
       </c>
       <c r="K185" s="28"/>
     </row>
-    <row r="186" spans="1:13">
+    <row r="186" spans="1:13" hidden="1">
       <c r="A186" s="19">
         <v>42975</v>
       </c>
@@ -15369,7 +15373,7 @@
       </c>
       <c r="K186" s="28"/>
     </row>
-    <row r="187" spans="1:13">
+    <row r="187" spans="1:13" hidden="1">
       <c r="A187" s="19">
         <v>42975</v>
       </c>
@@ -15397,7 +15401,7 @@
       </c>
       <c r="K187" s="28"/>
     </row>
-    <row r="188" spans="1:13">
+    <row r="188" spans="1:13" hidden="1">
       <c r="A188" s="19">
         <v>42975</v>
       </c>
@@ -15425,7 +15429,7 @@
       </c>
       <c r="K188" s="28"/>
     </row>
-    <row r="189" spans="1:13">
+    <row r="189" spans="1:13" hidden="1">
       <c r="A189" s="19">
         <v>42975</v>
       </c>
@@ -15464,7 +15468,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="190" spans="1:13">
+    <row r="190" spans="1:13" hidden="1">
       <c r="A190" s="19">
         <v>42975</v>
       </c>
@@ -15492,7 +15496,7 @@
       </c>
       <c r="K190" s="28"/>
     </row>
-    <row r="191" spans="1:13">
+    <row r="191" spans="1:13" hidden="1">
       <c r="A191" s="19">
         <v>42975</v>
       </c>
@@ -15531,7 +15535,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="192" spans="1:13">
+    <row r="192" spans="1:13" hidden="1">
       <c r="A192" s="19">
         <v>42975</v>
       </c>
@@ -15559,7 +15563,7 @@
       </c>
       <c r="K192" s="28"/>
     </row>
-    <row r="193" spans="1:13">
+    <row r="193" spans="1:13" hidden="1">
       <c r="A193" s="19">
         <v>42975</v>
       </c>
@@ -15598,7 +15602,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="194" spans="1:13">
+    <row r="194" spans="1:13" hidden="1">
       <c r="A194" s="19">
         <v>42975</v>
       </c>
@@ -15626,7 +15630,7 @@
       </c>
       <c r="K194" s="28"/>
     </row>
-    <row r="195" spans="1:13">
+    <row r="195" spans="1:13" hidden="1">
       <c r="A195" s="19">
         <v>42975</v>
       </c>
@@ -15657,7 +15661,7 @@
       </c>
       <c r="K195" s="28"/>
     </row>
-    <row r="196" spans="1:13">
+    <row r="196" spans="1:13" hidden="1">
       <c r="A196" s="19">
         <v>42975</v>
       </c>
@@ -15685,7 +15689,7 @@
       </c>
       <c r="K196" s="28"/>
     </row>
-    <row r="197" spans="1:13">
+    <row r="197" spans="1:13" hidden="1">
       <c r="A197" s="19">
         <v>42975</v>
       </c>
@@ -15724,7 +15728,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="198" spans="1:13">
+    <row r="198" spans="1:13" hidden="1">
       <c r="A198" s="19">
         <v>42975</v>
       </c>
@@ -15752,7 +15756,7 @@
       </c>
       <c r="K198" s="28"/>
     </row>
-    <row r="199" spans="1:13">
+    <row r="199" spans="1:13" hidden="1">
       <c r="A199" s="19">
         <v>42975</v>
       </c>
@@ -15791,7 +15795,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="200" spans="1:13">
+    <row r="200" spans="1:13" hidden="1">
       <c r="A200" s="19">
         <v>42975</v>
       </c>
@@ -15830,7 +15834,7 @@
         <v>1120</v>
       </c>
     </row>
-    <row r="201" spans="1:13">
+    <row r="201" spans="1:13" hidden="1">
       <c r="A201" s="19">
         <v>42975</v>
       </c>
@@ -15858,7 +15862,7 @@
       </c>
       <c r="K201" s="28"/>
     </row>
-    <row r="202" spans="1:13">
+    <row r="202" spans="1:13" hidden="1">
       <c r="A202" s="19">
         <v>42975</v>
       </c>
@@ -15897,7 +15901,7 @@
         <v>1124</v>
       </c>
     </row>
-    <row r="203" spans="1:13">
+    <row r="203" spans="1:13" hidden="1">
       <c r="A203" s="19">
         <v>42975</v>
       </c>
@@ -15925,7 +15929,7 @@
       </c>
       <c r="K203" s="28"/>
     </row>
-    <row r="204" spans="1:13">
+    <row r="204" spans="1:13" hidden="1">
       <c r="A204" s="19">
         <v>42975</v>
       </c>
@@ -15964,7 +15968,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="205" spans="1:13">
+    <row r="205" spans="1:13" hidden="1">
       <c r="A205" s="19">
         <v>42975</v>
       </c>
@@ -15992,7 +15996,7 @@
       </c>
       <c r="K205" s="28"/>
     </row>
-    <row r="206" spans="1:13">
+    <row r="206" spans="1:13" hidden="1">
       <c r="A206" s="19">
         <v>42975</v>
       </c>
@@ -16020,7 +16024,7 @@
       </c>
       <c r="K206" s="28"/>
     </row>
-    <row r="207" spans="1:13">
+    <row r="207" spans="1:13" hidden="1">
       <c r="A207" s="19">
         <v>42975</v>
       </c>
@@ -16059,7 +16063,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="208" spans="1:13">
+    <row r="208" spans="1:13" hidden="1">
       <c r="A208" s="19">
         <v>42975</v>
       </c>
@@ -16087,7 +16091,7 @@
       </c>
       <c r="K208" s="28"/>
     </row>
-    <row r="209" spans="1:13">
+    <row r="209" spans="1:13" hidden="1">
       <c r="A209" s="19">
         <v>42975</v>
       </c>
@@ -16115,7 +16119,7 @@
       </c>
       <c r="K209" s="28"/>
     </row>
-    <row r="210" spans="1:13">
+    <row r="210" spans="1:13" hidden="1">
       <c r="A210" s="19">
         <v>42975</v>
       </c>
@@ -16143,7 +16147,7 @@
       </c>
       <c r="K210" s="28"/>
     </row>
-    <row r="211" spans="1:13">
+    <row r="211" spans="1:13" hidden="1">
       <c r="A211" s="19">
         <v>42975</v>
       </c>
@@ -16171,7 +16175,7 @@
       </c>
       <c r="K211" s="28"/>
     </row>
-    <row r="212" spans="1:13">
+    <row r="212" spans="1:13" hidden="1">
       <c r="A212" s="19">
         <v>42975</v>
       </c>
@@ -16199,7 +16203,7 @@
       </c>
       <c r="K212" s="28"/>
     </row>
-    <row r="213" spans="1:13">
+    <row r="213" spans="1:13" hidden="1">
       <c r="A213" s="19">
         <v>42975</v>
       </c>
@@ -16227,7 +16231,7 @@
       </c>
       <c r="K213" s="28"/>
     </row>
-    <row r="214" spans="1:13">
+    <row r="214" spans="1:13" hidden="1">
       <c r="A214" s="19">
         <v>42975</v>
       </c>
@@ -16255,7 +16259,7 @@
       </c>
       <c r="K214" s="28"/>
     </row>
-    <row r="215" spans="1:13">
+    <row r="215" spans="1:13" hidden="1">
       <c r="A215" s="19">
         <v>42975</v>
       </c>
@@ -16283,7 +16287,7 @@
       </c>
       <c r="K215" s="28"/>
     </row>
-    <row r="216" spans="1:13">
+    <row r="216" spans="1:13" hidden="1">
       <c r="A216" s="19">
         <v>42975</v>
       </c>
@@ -16311,7 +16315,7 @@
       </c>
       <c r="K216" s="28"/>
     </row>
-    <row r="217" spans="1:13">
+    <row r="217" spans="1:13" hidden="1">
       <c r="A217" s="19">
         <v>42975</v>
       </c>
@@ -16350,7 +16354,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="218" spans="1:13">
+    <row r="218" spans="1:13" hidden="1">
       <c r="A218" s="19">
         <v>42975</v>
       </c>
@@ -16378,7 +16382,7 @@
       </c>
       <c r="K218" s="28"/>
     </row>
-    <row r="219" spans="1:13">
+    <row r="219" spans="1:13" hidden="1">
       <c r="A219" s="19">
         <v>42975</v>
       </c>
@@ -16406,7 +16410,7 @@
       </c>
       <c r="K219" s="28"/>
     </row>
-    <row r="220" spans="1:13">
+    <row r="220" spans="1:13" hidden="1">
       <c r="A220" s="19">
         <v>42975</v>
       </c>
@@ -16426,7 +16430,7 @@
         <v>4500</v>
       </c>
     </row>
-    <row r="221" spans="1:13">
+    <row r="221" spans="1:13" hidden="1">
       <c r="A221" s="19">
         <v>42975</v>
       </c>
@@ -16456,7 +16460,7 @@
       <c r="J221" s="32"/>
       <c r="K221" s="28"/>
     </row>
-    <row r="222" spans="1:13">
+    <row r="222" spans="1:13" hidden="1">
       <c r="A222" s="19">
         <v>42975</v>
       </c>
@@ -16486,7 +16490,7 @@
       <c r="J222" s="32"/>
       <c r="K222" s="28"/>
     </row>
-    <row r="223" spans="1:13">
+    <row r="223" spans="1:13" hidden="1">
       <c r="A223" s="19">
         <v>42975</v>
       </c>
@@ -16526,7 +16530,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="224" spans="1:13">
+    <row r="224" spans="1:13" hidden="1">
       <c r="A224" s="19">
         <v>42975</v>
       </c>
@@ -16556,7 +16560,7 @@
       <c r="J224" s="32"/>
       <c r="K224" s="28"/>
     </row>
-    <row r="225" spans="1:13">
+    <row r="225" spans="1:13" hidden="1">
       <c r="A225" s="19">
         <v>42975</v>
       </c>
@@ -16596,7 +16600,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="226" spans="1:13">
+    <row r="226" spans="1:13" hidden="1">
       <c r="A226" s="19">
         <v>42975</v>
       </c>
@@ -16626,7 +16630,7 @@
       <c r="J226" s="32"/>
       <c r="K226" s="28"/>
     </row>
-    <row r="227" spans="1:13">
+    <row r="227" spans="1:13" hidden="1">
       <c r="A227" s="19">
         <v>42975</v>
       </c>
@@ -16666,7 +16670,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="228" spans="1:13">
+    <row r="228" spans="1:13" hidden="1">
       <c r="A228" s="19">
         <v>42975</v>
       </c>
@@ -16696,7 +16700,7 @@
       <c r="J228" s="32"/>
       <c r="K228" s="28"/>
     </row>
-    <row r="229" spans="1:13">
+    <row r="229" spans="1:13" hidden="1">
       <c r="A229" s="19">
         <v>42975</v>
       </c>
@@ -16736,7 +16740,7 @@
         <v>1138</v>
       </c>
     </row>
-    <row r="230" spans="1:13">
+    <row r="230" spans="1:13" hidden="1">
       <c r="A230" s="19">
         <v>42975</v>
       </c>
@@ -16766,7 +16770,7 @@
       <c r="J230" s="32"/>
       <c r="K230" s="28"/>
     </row>
-    <row r="231" spans="1:13">
+    <row r="231" spans="1:13" hidden="1">
       <c r="A231" s="19">
         <v>42975</v>
       </c>
@@ -16806,7 +16810,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="232" spans="1:13">
+    <row r="232" spans="1:13" hidden="1">
       <c r="A232" s="19">
         <v>42975</v>
       </c>
@@ -16836,7 +16840,7 @@
       <c r="J232" s="32"/>
       <c r="K232" s="28"/>
     </row>
-    <row r="233" spans="1:13">
+    <row r="233" spans="1:13" hidden="1">
       <c r="A233" s="19">
         <v>42975</v>
       </c>
@@ -16876,7 +16880,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="234" spans="1:13">
+    <row r="234" spans="1:13" hidden="1">
       <c r="A234" s="19">
         <v>42975</v>
       </c>
@@ -16916,7 +16920,7 @@
         <v>971</v>
       </c>
     </row>
-    <row r="235" spans="1:13">
+    <row r="235" spans="1:13" hidden="1">
       <c r="A235" s="19">
         <v>42975</v>
       </c>
@@ -16956,7 +16960,7 @@
         <v>1139</v>
       </c>
     </row>
-    <row r="236" spans="1:13">
+    <row r="236" spans="1:13" hidden="1">
       <c r="A236" s="19">
         <v>42975</v>
       </c>
@@ -16986,7 +16990,7 @@
       <c r="J236" s="32"/>
       <c r="K236" s="28"/>
     </row>
-    <row r="237" spans="1:13">
+    <row r="237" spans="1:13" hidden="1">
       <c r="A237" s="19">
         <v>42975</v>
       </c>
@@ -17016,7 +17020,7 @@
       <c r="J237" s="32"/>
       <c r="K237" s="28"/>
     </row>
-    <row r="238" spans="1:13">
+    <row r="238" spans="1:13" hidden="1">
       <c r="A238" s="19">
         <v>42975</v>
       </c>
@@ -17046,7 +17050,7 @@
       <c r="J238" s="32"/>
       <c r="K238" s="28"/>
     </row>
-    <row r="239" spans="1:13">
+    <row r="239" spans="1:13" hidden="1">
       <c r="A239" s="19">
         <v>42975</v>
       </c>
@@ -17076,7 +17080,7 @@
       <c r="J239" s="32"/>
       <c r="K239" s="28"/>
     </row>
-    <row r="240" spans="1:13">
+    <row r="240" spans="1:13" hidden="1">
       <c r="A240" s="19">
         <v>42975</v>
       </c>
@@ -17106,7 +17110,7 @@
       <c r="J240" s="32"/>
       <c r="K240" s="28"/>
     </row>
-    <row r="241" spans="1:13">
+    <row r="241" spans="1:13" hidden="1">
       <c r="A241" s="19">
         <v>42975</v>
       </c>
@@ -17146,7 +17150,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="242" spans="1:13">
+    <row r="242" spans="1:13" hidden="1">
       <c r="A242" s="19">
         <v>42975</v>
       </c>
@@ -17176,7 +17180,7 @@
       <c r="J242" s="32"/>
       <c r="K242" s="28"/>
     </row>
-    <row r="243" spans="1:13">
+    <row r="243" spans="1:13" hidden="1">
       <c r="A243" s="19">
         <v>42975</v>
       </c>
@@ -17206,7 +17210,7 @@
       <c r="J243" s="32"/>
       <c r="K243" s="28"/>
     </row>
-    <row r="244" spans="1:13">
+    <row r="244" spans="1:13" hidden="1">
       <c r="A244" s="19">
         <v>42975</v>
       </c>
@@ -17236,7 +17240,7 @@
       <c r="J244" s="32"/>
       <c r="K244" s="28"/>
     </row>
-    <row r="245" spans="1:13">
+    <row r="245" spans="1:13" hidden="1">
       <c r="A245" s="19">
         <v>42975</v>
       </c>
@@ -17276,7 +17280,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="246" spans="1:13">
+    <row r="246" spans="1:13" hidden="1">
       <c r="A246" s="19">
         <v>42975</v>
       </c>
@@ -17306,7 +17310,7 @@
       <c r="J246" s="32"/>
       <c r="K246" s="28"/>
     </row>
-    <row r="247" spans="1:13">
+    <row r="247" spans="1:13" hidden="1">
       <c r="A247" s="19">
         <v>42975</v>
       </c>
@@ -17336,7 +17340,7 @@
       <c r="J247" s="32"/>
       <c r="K247" s="28"/>
     </row>
-    <row r="248" spans="1:13">
+    <row r="248" spans="1:13" hidden="1">
       <c r="A248" s="19">
         <v>42975</v>
       </c>
@@ -17366,7 +17370,7 @@
       <c r="J248" s="32"/>
       <c r="K248" s="28"/>
     </row>
-    <row r="249" spans="1:13">
+    <row r="249" spans="1:13" hidden="1">
       <c r="A249" s="19">
         <v>42975</v>
       </c>
@@ -17396,7 +17400,7 @@
       <c r="J249" s="32"/>
       <c r="K249" s="28"/>
     </row>
-    <row r="250" spans="1:13">
+    <row r="250" spans="1:13" hidden="1">
       <c r="A250" s="19">
         <v>42975</v>
       </c>
@@ -17426,7 +17430,7 @@
       <c r="J250" s="32"/>
       <c r="K250" s="28"/>
     </row>
-    <row r="251" spans="1:13">
+    <row r="251" spans="1:13" hidden="1">
       <c r="A251" s="19">
         <v>42975</v>
       </c>
@@ -17456,7 +17460,7 @@
       <c r="J251" s="35"/>
       <c r="K251" s="36"/>
     </row>
-    <row r="252" spans="1:13">
+    <row r="252" spans="1:13" hidden="1">
       <c r="A252" s="19">
         <v>42975</v>
       </c>
@@ -17486,7 +17490,7 @@
       <c r="J252" s="32"/>
       <c r="K252" s="28"/>
     </row>
-    <row r="253" spans="1:13">
+    <row r="253" spans="1:13" hidden="1">
       <c r="A253" s="19">
         <v>42975</v>
       </c>
@@ -17516,7 +17520,7 @@
       <c r="J253" s="35"/>
       <c r="K253" s="36"/>
     </row>
-    <row r="254" spans="1:13">
+    <row r="254" spans="1:13" hidden="1">
       <c r="A254" s="19">
         <v>42975</v>
       </c>
@@ -17546,7 +17550,7 @@
       <c r="J254" s="32"/>
       <c r="K254" s="28"/>
     </row>
-    <row r="255" spans="1:13">
+    <row r="255" spans="1:13" hidden="1">
       <c r="A255" s="19">
         <v>42975</v>
       </c>
@@ -17586,7 +17590,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="256" spans="1:13">
+    <row r="256" spans="1:13" hidden="1">
       <c r="A256" s="19">
         <v>42975</v>
       </c>
@@ -17616,7 +17620,7 @@
       <c r="J256" s="32"/>
       <c r="K256" s="28"/>
     </row>
-    <row r="257" spans="1:13">
+    <row r="257" spans="1:13" hidden="1">
       <c r="A257" s="19">
         <v>42975</v>
       </c>
@@ -17648,7 +17652,7 @@
       <c r="J257" s="32"/>
       <c r="K257" s="28"/>
     </row>
-    <row r="258" spans="1:13">
+    <row r="258" spans="1:13" hidden="1">
       <c r="A258" s="19">
         <v>42975</v>
       </c>
@@ -17678,7 +17682,7 @@
       <c r="J258" s="32"/>
       <c r="K258" s="28"/>
     </row>
-    <row r="259" spans="1:13">
+    <row r="259" spans="1:13" hidden="1">
       <c r="A259" s="19">
         <v>42975</v>
       </c>
@@ -17708,7 +17712,7 @@
       <c r="J259" s="32"/>
       <c r="K259" s="28"/>
     </row>
-    <row r="260" spans="1:13">
+    <row r="260" spans="1:13" hidden="1">
       <c r="A260" s="19">
         <v>42975</v>
       </c>
@@ -17738,7 +17742,7 @@
       <c r="J260" s="32"/>
       <c r="K260" s="28"/>
     </row>
-    <row r="261" spans="1:13">
+    <row r="261" spans="1:13" hidden="1">
       <c r="A261" s="19">
         <v>42975</v>
       </c>
@@ -17768,7 +17772,7 @@
       <c r="J261" s="32"/>
       <c r="K261" s="28"/>
     </row>
-    <row r="262" spans="1:13">
+    <row r="262" spans="1:13" hidden="1">
       <c r="A262" s="19">
         <v>42975</v>
       </c>
@@ -17798,7 +17802,7 @@
       <c r="J262" s="32"/>
       <c r="K262" s="28"/>
     </row>
-    <row r="263" spans="1:13">
+    <row r="263" spans="1:13" hidden="1">
       <c r="A263" s="19">
         <v>42975</v>
       </c>
@@ -17838,7 +17842,7 @@
         <v>1138</v>
       </c>
     </row>
-    <row r="264" spans="1:13">
+    <row r="264" spans="1:13" hidden="1">
       <c r="A264" s="19">
         <v>42975</v>
       </c>
@@ -17868,7 +17872,7 @@
       <c r="J264" s="32"/>
       <c r="K264" s="28"/>
     </row>
-    <row r="265" spans="1:13">
+    <row r="265" spans="1:13" hidden="1">
       <c r="A265" s="19">
         <v>42975</v>
       </c>
@@ -17898,7 +17902,7 @@
       <c r="J265" s="32"/>
       <c r="K265" s="28"/>
     </row>
-    <row r="266" spans="1:13">
+    <row r="266" spans="1:13" hidden="1">
       <c r="A266" s="19">
         <v>42975</v>
       </c>
@@ -17925,7 +17929,7 @@
       <c r="J266" s="35"/>
       <c r="K266" s="36"/>
     </row>
-    <row r="267" spans="1:13">
+    <row r="267" spans="1:13" hidden="1">
       <c r="A267" s="19">
         <v>42975</v>
       </c>
@@ -17952,7 +17956,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="268" spans="1:13">
+    <row r="268" spans="1:13" hidden="1">
       <c r="A268" s="19">
         <v>42975</v>
       </c>
@@ -17979,7 +17983,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="269" spans="1:13">
+    <row r="269" spans="1:13" hidden="1">
       <c r="A269" s="19">
         <v>42975</v>
       </c>
@@ -18006,7 +18010,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="270" spans="1:13">
+    <row r="270" spans="1:13" hidden="1">
       <c r="A270" s="19">
         <v>42975</v>
       </c>
@@ -18045,7 +18049,7 @@
         <v>1143</v>
       </c>
     </row>
-    <row r="271" spans="1:13">
+    <row r="271" spans="1:13" hidden="1">
       <c r="A271" s="19">
         <v>42975</v>
       </c>
@@ -18084,7 +18088,7 @@
         <v>1120</v>
       </c>
     </row>
-    <row r="272" spans="1:13">
+    <row r="272" spans="1:13" hidden="1">
       <c r="A272" s="19">
         <v>42975</v>
       </c>
@@ -18111,7 +18115,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="273" spans="1:13">
+    <row r="273" spans="1:13" hidden="1">
       <c r="A273" s="19">
         <v>42975</v>
       </c>
@@ -18150,7 +18154,7 @@
         <v>1144</v>
       </c>
     </row>
-    <row r="274" spans="1:13">
+    <row r="274" spans="1:13" hidden="1">
       <c r="A274" s="19">
         <v>42975</v>
       </c>
@@ -18177,7 +18181,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="275" spans="1:13">
+    <row r="275" spans="1:13" hidden="1">
       <c r="A275" s="19">
         <v>42975</v>
       </c>
@@ -18207,7 +18211,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="276" spans="1:13">
+    <row r="276" spans="1:13" hidden="1">
       <c r="A276" s="19">
         <v>42975</v>
       </c>
@@ -18234,7 +18238,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="277" spans="1:13">
+    <row r="277" spans="1:13" hidden="1">
       <c r="A277" s="19">
         <v>42975</v>
       </c>
@@ -18273,7 +18277,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="278" spans="1:13">
+    <row r="278" spans="1:13" hidden="1">
       <c r="A278" s="19">
         <v>42975</v>
       </c>
@@ -18300,7 +18304,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="279" spans="1:13">
+    <row r="279" spans="1:13" hidden="1">
       <c r="A279" s="19">
         <v>42975</v>
       </c>
@@ -18336,7 +18340,7 @@
         <v>1130</v>
       </c>
     </row>
-    <row r="280" spans="1:13">
+    <row r="280" spans="1:13" hidden="1">
       <c r="A280" s="19">
         <v>42975</v>
       </c>
@@ -18375,7 +18379,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="281" spans="1:13">
+    <row r="281" spans="1:13" hidden="1">
       <c r="A281" s="19">
         <v>42975</v>
       </c>
@@ -18402,7 +18406,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="282" spans="1:13">
+    <row r="282" spans="1:13" hidden="1">
       <c r="A282" s="19">
         <v>42975</v>
       </c>
@@ -18441,7 +18445,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="283" spans="1:13">
+    <row r="283" spans="1:13" hidden="1">
       <c r="A283" s="19">
         <v>42975</v>
       </c>
@@ -18468,7 +18472,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="284" spans="1:13">
+    <row r="284" spans="1:13" hidden="1">
       <c r="A284" s="19">
         <v>42975</v>
       </c>
@@ -18495,7 +18499,7 @@
         <v>923</v>
       </c>
     </row>
-    <row r="285" spans="1:13">
+    <row r="285" spans="1:13" hidden="1">
       <c r="A285" s="19">
         <v>42975</v>
       </c>
@@ -18534,7 +18538,7 @@
         <v>1143</v>
       </c>
     </row>
-    <row r="286" spans="1:13">
+    <row r="286" spans="1:13" hidden="1">
       <c r="A286" s="19">
         <v>42975</v>
       </c>
@@ -18561,7 +18565,7 @@
         <v>923</v>
       </c>
     </row>
-    <row r="287" spans="1:13">
+    <row r="287" spans="1:13" hidden="1">
       <c r="A287" s="19">
         <v>42975</v>
       </c>
@@ -18588,7 +18592,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="288" spans="1:13">
+    <row r="288" spans="1:13" hidden="1">
       <c r="A288" s="19">
         <v>42975</v>
       </c>
@@ -18615,7 +18619,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="289" spans="1:13">
+    <row r="289" spans="1:13" hidden="1">
       <c r="A289" s="19">
         <v>42975</v>
       </c>
@@ -18642,7 +18646,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="290" spans="1:13">
+    <row r="290" spans="1:13" hidden="1">
       <c r="A290" s="19">
         <v>42975</v>
       </c>
@@ -18669,7 +18673,7 @@
         <v>923</v>
       </c>
     </row>
-    <row r="291" spans="1:13">
+    <row r="291" spans="1:13" hidden="1">
       <c r="A291" s="19">
         <v>42975</v>
       </c>
@@ -18696,7 +18700,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="292" spans="1:13">
+    <row r="292" spans="1:13" hidden="1">
       <c r="A292" s="19">
         <v>42975</v>
       </c>
@@ -18723,7 +18727,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="293" spans="1:13">
+    <row r="293" spans="1:13" hidden="1">
       <c r="A293" s="19">
         <v>42975</v>
       </c>
@@ -18750,7 +18754,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="294" spans="1:13">
+    <row r="294" spans="1:13" hidden="1">
       <c r="A294" s="19">
         <v>42975</v>
       </c>
@@ -18777,7 +18781,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="295" spans="1:13">
+    <row r="295" spans="1:13" hidden="1">
       <c r="A295" s="19">
         <v>42975</v>
       </c>
@@ -18807,7 +18811,7 @@
         <v>925</v>
       </c>
     </row>
-    <row r="296" spans="1:13">
+    <row r="296" spans="1:13" hidden="1">
       <c r="A296" s="19">
         <v>42975</v>
       </c>
@@ -18834,7 +18838,7 @@
         <v>923</v>
       </c>
     </row>
-    <row r="297" spans="1:13">
+    <row r="297" spans="1:13" hidden="1">
       <c r="A297" s="19">
         <v>42975</v>
       </c>
@@ -18864,7 +18868,7 @@
         <v>925</v>
       </c>
     </row>
-    <row r="298" spans="1:13">
+    <row r="298" spans="1:13" hidden="1">
       <c r="A298" s="19">
         <v>42975</v>
       </c>
@@ -18891,7 +18895,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="299" spans="1:13">
+    <row r="299" spans="1:13" hidden="1">
       <c r="A299" s="19">
         <v>42975</v>
       </c>
@@ -18921,7 +18925,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="300" spans="1:13">
+    <row r="300" spans="1:13" hidden="1">
       <c r="A300" s="19">
         <v>42975</v>
       </c>
@@ -18948,7 +18952,7 @@
         <v>923</v>
       </c>
     </row>
-    <row r="301" spans="1:13">
+    <row r="301" spans="1:13" hidden="1">
       <c r="A301" s="19">
         <v>42975</v>
       </c>
@@ -18975,7 +18979,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="302" spans="1:13">
+    <row r="302" spans="1:13" hidden="1">
       <c r="A302" s="19">
         <v>42975</v>
       </c>
@@ -19002,7 +19006,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="303" spans="1:13">
+    <row r="303" spans="1:13" hidden="1">
       <c r="A303" s="19">
         <v>42975</v>
       </c>
@@ -19029,7 +19033,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="304" spans="1:13">
+    <row r="304" spans="1:13" hidden="1">
       <c r="A304" s="19">
         <v>42975</v>
       </c>
@@ -19068,7 +19072,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="305" spans="1:13">
+    <row r="305" spans="1:13" hidden="1">
       <c r="A305" s="19">
         <v>42975</v>
       </c>
@@ -19095,7 +19099,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="306" spans="1:13">
+    <row r="306" spans="1:13" hidden="1">
       <c r="A306" s="19">
         <v>42975</v>
       </c>
@@ -19122,7 +19126,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="307" spans="1:13">
+    <row r="307" spans="1:13" hidden="1">
       <c r="A307" s="19">
         <v>42975</v>
       </c>
@@ -19149,7 +19153,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="308" spans="1:13">
+    <row r="308" spans="1:13" hidden="1">
       <c r="A308" s="19">
         <v>42975</v>
       </c>
@@ -19179,7 +19183,7 @@
         <v>925</v>
       </c>
     </row>
-    <row r="309" spans="1:13">
+    <row r="309" spans="1:13" hidden="1">
       <c r="A309" s="19">
         <v>42975</v>
       </c>
@@ -19206,7 +19210,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="310" spans="1:13">
+    <row r="310" spans="1:13" hidden="1">
       <c r="A310" s="19">
         <v>42975</v>
       </c>
@@ -19236,7 +19240,7 @@
         <v>925</v>
       </c>
     </row>
-    <row r="311" spans="1:13">
+    <row r="311" spans="1:13" hidden="1">
       <c r="A311" s="19">
         <v>42975</v>
       </c>
@@ -19263,7 +19267,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="312" spans="1:13">
+    <row r="312" spans="1:13" hidden="1">
       <c r="A312" s="19">
         <v>42975</v>
       </c>
@@ -19293,7 +19297,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="313" spans="1:13">
+    <row r="313" spans="1:13" hidden="1">
       <c r="A313" s="19">
         <v>42975</v>
       </c>
@@ -19320,7 +19324,7 @@
         <v>923</v>
       </c>
     </row>
-    <row r="314" spans="1:13">
+    <row r="314" spans="1:13" hidden="1">
       <c r="A314" s="19">
         <v>42975</v>
       </c>
@@ -19350,7 +19354,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="315" spans="1:13">
+    <row r="315" spans="1:13" hidden="1">
       <c r="A315" s="19">
         <v>42975</v>
       </c>
@@ -19377,7 +19381,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="316" spans="1:13">
+    <row r="316" spans="1:13" hidden="1">
       <c r="A316" s="19">
         <v>42975</v>
       </c>
@@ -19407,7 +19411,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="317" spans="1:13">
+    <row r="317" spans="1:13" hidden="1">
       <c r="A317" s="19">
         <v>42975</v>
       </c>
@@ -19434,7 +19438,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="318" spans="1:13">
+    <row r="318" spans="1:13" hidden="1">
       <c r="A318" s="19">
         <v>42975</v>
       </c>
@@ -19473,7 +19477,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="319" spans="1:13">
+    <row r="319" spans="1:13" hidden="1">
       <c r="A319" s="19">
         <v>42975</v>
       </c>
@@ -19500,7 +19504,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="320" spans="1:13">
+    <row r="320" spans="1:13" hidden="1">
       <c r="A320" s="19">
         <v>42975</v>
       </c>
@@ -19539,7 +19543,7 @@
         <v>1131</v>
       </c>
     </row>
-    <row r="321" spans="1:13">
+    <row r="321" spans="1:13" hidden="1">
       <c r="A321" s="19">
         <v>42975</v>
       </c>
@@ -19569,7 +19573,7 @@
         <v>925</v>
       </c>
     </row>
-    <row r="322" spans="1:13">
+    <row r="322" spans="1:13" hidden="1">
       <c r="A322" s="19">
         <v>42975</v>
       </c>
@@ -19596,7 +19600,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="323" spans="1:13">
+    <row r="323" spans="1:13" hidden="1">
       <c r="A323" s="19">
         <v>42975</v>
       </c>
@@ -19635,7 +19639,7 @@
         <v>1124</v>
       </c>
     </row>
-    <row r="324" spans="1:13">
+    <row r="324" spans="1:13" hidden="1">
       <c r="A324" s="19">
         <v>42975</v>
       </c>
@@ -19674,7 +19678,7 @@
         <v>1124</v>
       </c>
     </row>
-    <row r="325" spans="1:13">
+    <row r="325" spans="1:13" hidden="1">
       <c r="A325" s="19">
         <v>42975</v>
       </c>
@@ -19701,7 +19705,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="326" spans="1:13">
+    <row r="326" spans="1:13" hidden="1">
       <c r="A326" s="19">
         <v>42975</v>
       </c>
@@ -19728,7 +19732,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="327" spans="1:13">
+    <row r="327" spans="1:13" hidden="1">
       <c r="A327" s="19">
         <v>42975</v>
       </c>
@@ -19767,7 +19771,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="328" spans="1:13">
+    <row r="328" spans="1:13" hidden="1">
       <c r="A328" s="19">
         <v>42975</v>
       </c>
@@ -19794,7 +19798,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="329" spans="1:13">
+    <row r="329" spans="1:13" hidden="1">
       <c r="A329" s="19">
         <v>42975</v>
       </c>
@@ -19821,7 +19825,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="330" spans="1:13">
+    <row r="330" spans="1:13" hidden="1">
       <c r="A330" s="19">
         <v>42975</v>
       </c>
@@ -19860,7 +19864,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="331" spans="1:13">
+    <row r="331" spans="1:13" hidden="1">
       <c r="A331" s="19">
         <v>42975</v>
       </c>
@@ -19887,7 +19891,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="332" spans="1:13">
+    <row r="332" spans="1:13" hidden="1">
       <c r="A332" s="19">
         <v>42975</v>
       </c>
@@ -19926,7 +19930,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="333" spans="1:13">
+    <row r="333" spans="1:13" hidden="1">
       <c r="A333" s="19">
         <v>42975</v>
       </c>
@@ -19953,7 +19957,7 @@
         <v>923</v>
       </c>
     </row>
-    <row r="334" spans="1:13">
+    <row r="334" spans="1:13" hidden="1">
       <c r="A334" s="19">
         <v>42975</v>
       </c>
@@ -19992,7 +19996,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="335" spans="1:13">
+    <row r="335" spans="1:13" hidden="1">
       <c r="A335" s="19">
         <v>42975</v>
       </c>
@@ -20019,7 +20023,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="336" spans="1:13">
+    <row r="336" spans="1:13" hidden="1">
       <c r="A336" s="19">
         <v>42975</v>
       </c>
@@ -20046,7 +20050,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="337" spans="1:13">
+    <row r="337" spans="1:13" hidden="1">
       <c r="A337" s="19">
         <v>42975</v>
       </c>
@@ -20076,7 +20080,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="338" spans="1:13">
+    <row r="338" spans="1:13" hidden="1">
       <c r="A338" s="19">
         <v>42975</v>
       </c>
@@ -20115,7 +20119,7 @@
         <v>1031</v>
       </c>
     </row>
-    <row r="339" spans="1:13">
+    <row r="339" spans="1:13" hidden="1">
       <c r="A339" s="19">
         <v>42975</v>
       </c>
@@ -20142,7 +20146,7 @@
         <v>923</v>
       </c>
     </row>
-    <row r="340" spans="1:13">
+    <row r="340" spans="1:13" hidden="1">
       <c r="A340" s="19">
         <v>42975</v>
       </c>
@@ -20169,7 +20173,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="341" spans="1:13">
+    <row r="341" spans="1:13" hidden="1">
       <c r="A341" s="19">
         <v>42975</v>
       </c>
@@ -20199,7 +20203,7 @@
         <v>925</v>
       </c>
     </row>
-    <row r="342" spans="1:13">
+    <row r="342" spans="1:13" hidden="1">
       <c r="A342" s="19">
         <v>42975</v>
       </c>
@@ -20226,7 +20230,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="343" spans="1:13">
+    <row r="343" spans="1:13" hidden="1">
       <c r="A343" s="19">
         <v>42975</v>
       </c>
@@ -20259,7 +20263,7 @@
         <v>1670</v>
       </c>
     </row>
-    <row r="344" spans="1:13">
+    <row r="344" spans="1:13" hidden="1">
       <c r="A344" s="19">
         <v>42975</v>
       </c>
@@ -20286,7 +20290,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="345" spans="1:13">
+    <row r="345" spans="1:13" hidden="1">
       <c r="A345" s="19">
         <v>42975</v>
       </c>
@@ -20313,7 +20317,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="346" spans="1:13">
+    <row r="346" spans="1:13" hidden="1">
       <c r="A346" s="19">
         <v>42975</v>
       </c>
@@ -20352,7 +20356,7 @@
         <v>1132</v>
       </c>
     </row>
-    <row r="347" spans="1:13">
+    <row r="347" spans="1:13" hidden="1">
       <c r="A347" s="19">
         <v>42975</v>
       </c>
@@ -20382,7 +20386,7 @@
         <v>925</v>
       </c>
     </row>
-    <row r="348" spans="1:13">
+    <row r="348" spans="1:13" hidden="1">
       <c r="A348" s="19">
         <v>42975</v>
       </c>
@@ -20409,7 +20413,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="349" spans="1:13">
+    <row r="349" spans="1:13" hidden="1">
       <c r="A349" s="19">
         <v>42975</v>
       </c>
@@ -20439,7 +20443,7 @@
         <v>925</v>
       </c>
     </row>
-    <row r="350" spans="1:13">
+    <row r="350" spans="1:13" hidden="1">
       <c r="A350" s="19">
         <v>42975</v>
       </c>
@@ -20466,7 +20470,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="351" spans="1:13">
+    <row r="351" spans="1:13" hidden="1">
       <c r="A351" s="19">
         <v>42975</v>
       </c>
@@ -20505,7 +20509,7 @@
         <v>1120</v>
       </c>
     </row>
-    <row r="352" spans="1:13">
+    <row r="352" spans="1:13" hidden="1">
       <c r="A352" s="19">
         <v>42975</v>
       </c>
@@ -20535,7 +20539,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="353" spans="1:13">
+    <row r="353" spans="1:13" hidden="1">
       <c r="A353" s="19">
         <v>42975</v>
       </c>
@@ -20565,7 +20569,7 @@
         <v>942</v>
       </c>
     </row>
-    <row r="354" spans="1:13">
+    <row r="354" spans="1:13" hidden="1">
       <c r="A354" s="19">
         <v>42975</v>
       </c>
@@ -20592,7 +20596,7 @@
         <v>923</v>
       </c>
     </row>
-    <row r="355" spans="1:13">
+    <row r="355" spans="1:13" hidden="1">
       <c r="A355" s="19">
         <v>42975</v>
       </c>
@@ -20631,7 +20635,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="356" spans="1:13">
+    <row r="356" spans="1:13" hidden="1">
       <c r="A356" s="19">
         <v>42975</v>
       </c>
@@ -20670,7 +20674,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="357" spans="1:13">
+    <row r="357" spans="1:13" hidden="1">
       <c r="A357" s="19">
         <v>42975</v>
       </c>
@@ -20697,7 +20701,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="358" spans="1:13">
+    <row r="358" spans="1:13" hidden="1">
       <c r="A358" s="19">
         <v>42975</v>
       </c>
@@ -20736,7 +20740,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="359" spans="1:13">
+    <row r="359" spans="1:13" hidden="1">
       <c r="A359" s="19">
         <v>42975</v>
       </c>
@@ -20763,7 +20767,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="360" spans="1:13">
+    <row r="360" spans="1:13" hidden="1">
       <c r="A360" s="19">
         <v>42975</v>
       </c>
@@ -20790,7 +20794,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="361" spans="1:13">
+    <row r="361" spans="1:13" hidden="1">
       <c r="A361" s="19">
         <v>42975</v>
       </c>
@@ -20829,7 +20833,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="362" spans="1:13">
+    <row r="362" spans="1:13" hidden="1">
       <c r="A362" s="19">
         <v>42975</v>
       </c>
@@ -20856,7 +20860,7 @@
         <v>923</v>
       </c>
     </row>
-    <row r="363" spans="1:13">
+    <row r="363" spans="1:13" hidden="1">
       <c r="A363" s="19">
         <v>42975</v>
       </c>
@@ -20883,7 +20887,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="364" spans="1:13">
+    <row r="364" spans="1:13" hidden="1">
       <c r="A364" s="19">
         <v>42975</v>
       </c>
@@ -20913,7 +20917,7 @@
         <v>925</v>
       </c>
     </row>
-    <row r="365" spans="1:13">
+    <row r="365" spans="1:13" hidden="1">
       <c r="A365" s="19">
         <v>42975</v>
       </c>
@@ -20940,7 +20944,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="366" spans="1:13">
+    <row r="366" spans="1:13" hidden="1">
       <c r="A366" s="19">
         <v>42975</v>
       </c>
@@ -20979,7 +20983,7 @@
         <v>1121</v>
       </c>
     </row>
-    <row r="367" spans="1:13">
+    <row r="367" spans="1:13" hidden="1">
       <c r="A367" s="19">
         <v>42975</v>
       </c>
@@ -21006,7 +21010,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="368" spans="1:13">
+    <row r="368" spans="1:13" hidden="1">
       <c r="A368" s="19">
         <v>42975</v>
       </c>
@@ -21033,7 +21037,7 @@
         <v>923</v>
       </c>
     </row>
-    <row r="369" spans="1:13">
+    <row r="369" spans="1:13" hidden="1">
       <c r="A369" s="19">
         <v>42975</v>
       </c>
@@ -21063,7 +21067,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="370" spans="1:13">
+    <row r="370" spans="1:13" hidden="1">
       <c r="A370" s="19">
         <v>42975</v>
       </c>
@@ -21102,7 +21106,7 @@
         <v>1124</v>
       </c>
     </row>
-    <row r="371" spans="1:13">
+    <row r="371" spans="1:13" hidden="1">
       <c r="A371" s="19">
         <v>42975</v>
       </c>
@@ -21137,7 +21141,7 @@
         <v>1124</v>
       </c>
     </row>
-    <row r="372" spans="1:13">
+    <row r="372" spans="1:13" hidden="1">
       <c r="A372" s="19">
         <v>42975</v>
       </c>
@@ -21165,7 +21169,7 @@
       </c>
       <c r="J372" s="42"/>
     </row>
-    <row r="373" spans="1:13">
+    <row r="373" spans="1:13" hidden="1">
       <c r="A373" s="19">
         <v>42975</v>
       </c>
@@ -21204,7 +21208,7 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="374" spans="1:13">
+    <row r="374" spans="1:13" hidden="1">
       <c r="A374" s="19">
         <v>42975</v>
       </c>
@@ -21232,7 +21236,7 @@
       </c>
       <c r="J374" s="42"/>
     </row>
-    <row r="375" spans="1:13">
+    <row r="375" spans="1:13" hidden="1">
       <c r="A375" s="19">
         <v>42975</v>
       </c>
@@ -21260,7 +21264,7 @@
       </c>
       <c r="J375" s="42"/>
     </row>
-    <row r="376" spans="1:13">
+    <row r="376" spans="1:13" hidden="1">
       <c r="A376" s="19">
         <v>42975</v>
       </c>
@@ -21288,7 +21292,7 @@
       </c>
       <c r="J376" s="42"/>
     </row>
-    <row r="377" spans="1:13">
+    <row r="377" spans="1:13" hidden="1">
       <c r="A377" s="19">
         <v>42975</v>
       </c>
@@ -21316,7 +21320,7 @@
       </c>
       <c r="J377" s="42"/>
     </row>
-    <row r="378" spans="1:13">
+    <row r="378" spans="1:13" hidden="1">
       <c r="A378" s="19">
         <v>42975</v>
       </c>
@@ -21344,7 +21348,7 @@
       </c>
       <c r="J378" s="42"/>
     </row>
-    <row r="379" spans="1:13">
+    <row r="379" spans="1:13" hidden="1">
       <c r="A379" s="19">
         <v>42975</v>
       </c>
@@ -21383,7 +21387,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="380" spans="1:13">
+    <row r="380" spans="1:13" hidden="1">
       <c r="A380" s="19">
         <v>42975</v>
       </c>
@@ -21411,7 +21415,7 @@
       </c>
       <c r="J380" s="42"/>
     </row>
-    <row r="381" spans="1:13">
+    <row r="381" spans="1:13" hidden="1">
       <c r="A381" s="19">
         <v>42975</v>
       </c>
@@ -21439,7 +21443,7 @@
       </c>
       <c r="J381" s="42"/>
     </row>
-    <row r="382" spans="1:13">
+    <row r="382" spans="1:13" hidden="1">
       <c r="A382" s="19">
         <v>42975</v>
       </c>
@@ -21470,7 +21474,7 @@
       </c>
       <c r="J382" s="42"/>
     </row>
-    <row r="383" spans="1:13">
+    <row r="383" spans="1:13" hidden="1">
       <c r="A383" s="19">
         <v>42975</v>
       </c>
@@ -21509,7 +21513,7 @@
         <v>1121</v>
       </c>
     </row>
-    <row r="384" spans="1:13">
+    <row r="384" spans="1:13" hidden="1">
       <c r="A384" s="19">
         <v>42975</v>
       </c>
@@ -21540,7 +21544,7 @@
       </c>
       <c r="J384" s="42"/>
     </row>
-    <row r="385" spans="1:13">
+    <row r="385" spans="1:13" hidden="1">
       <c r="A385" s="19">
         <v>42975</v>
       </c>
@@ -21579,7 +21583,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="386" spans="1:13">
+    <row r="386" spans="1:13" hidden="1">
       <c r="A386" s="19">
         <v>42975</v>
       </c>
@@ -21607,7 +21611,7 @@
       </c>
       <c r="J386" s="42"/>
     </row>
-    <row r="387" spans="1:13">
+    <row r="387" spans="1:13" hidden="1">
       <c r="A387" s="19">
         <v>42975</v>
       </c>
@@ -21646,7 +21650,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="388" spans="1:13">
+    <row r="388" spans="1:13" hidden="1">
       <c r="A388" s="19">
         <v>42975</v>
       </c>
@@ -21685,7 +21689,7 @@
         <v>1132</v>
       </c>
     </row>
-    <row r="389" spans="1:13">
+    <row r="389" spans="1:13" hidden="1">
       <c r="A389" s="19">
         <v>42975</v>
       </c>
@@ -21724,7 +21728,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="390" spans="1:13">
+    <row r="390" spans="1:13" hidden="1">
       <c r="A390" s="19">
         <v>42975</v>
       </c>
@@ -21752,7 +21756,7 @@
       </c>
       <c r="J390" s="42"/>
     </row>
-    <row r="391" spans="1:13">
+    <row r="391" spans="1:13" hidden="1">
       <c r="A391" s="19">
         <v>42975</v>
       </c>
@@ -21791,7 +21795,7 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="392" spans="1:13">
+    <row r="392" spans="1:13" hidden="1">
       <c r="A392" s="19">
         <v>42975</v>
       </c>
@@ -21819,7 +21823,7 @@
       </c>
       <c r="J392" s="42"/>
     </row>
-    <row r="393" spans="1:13">
+    <row r="393" spans="1:13" hidden="1">
       <c r="A393" s="19">
         <v>42975</v>
       </c>
@@ -21858,7 +21862,7 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="394" spans="1:13">
+    <row r="394" spans="1:13" hidden="1">
       <c r="A394" s="19">
         <v>42975</v>
       </c>
@@ -21886,7 +21890,7 @@
       </c>
       <c r="J394" s="42"/>
     </row>
-    <row r="395" spans="1:13">
+    <row r="395" spans="1:13" hidden="1">
       <c r="A395" s="19">
         <v>42975</v>
       </c>
@@ -21914,7 +21918,7 @@
       </c>
       <c r="J395" s="42"/>
     </row>
-    <row r="396" spans="1:13">
+    <row r="396" spans="1:13" hidden="1">
       <c r="A396" s="19">
         <v>42975</v>
       </c>
@@ -21953,7 +21957,7 @@
         <v>1120</v>
       </c>
     </row>
-    <row r="397" spans="1:13">
+    <row r="397" spans="1:13" hidden="1">
       <c r="A397" s="19">
         <v>42975</v>
       </c>
@@ -21981,7 +21985,7 @@
       </c>
       <c r="J397" s="42"/>
     </row>
-    <row r="398" spans="1:13">
+    <row r="398" spans="1:13" hidden="1">
       <c r="A398" s="19">
         <v>42975</v>
       </c>
@@ -22020,7 +22024,7 @@
         <v>1132</v>
       </c>
     </row>
-    <row r="399" spans="1:13">
+    <row r="399" spans="1:13" hidden="1">
       <c r="A399" s="19">
         <v>42975</v>
       </c>
@@ -22048,7 +22052,7 @@
       </c>
       <c r="J399" s="42"/>
     </row>
-    <row r="400" spans="1:13">
+    <row r="400" spans="1:13" hidden="1">
       <c r="A400" s="19">
         <v>42975</v>
       </c>
@@ -22087,7 +22091,7 @@
         <v>1132</v>
       </c>
     </row>
-    <row r="401" spans="1:13">
+    <row r="401" spans="1:13" hidden="1">
       <c r="A401" s="19">
         <v>42975</v>
       </c>
@@ -22126,7 +22130,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="402" spans="1:13">
+    <row r="402" spans="1:13" hidden="1">
       <c r="A402" s="19">
         <v>42975</v>
       </c>
@@ -22154,7 +22158,7 @@
       </c>
       <c r="J402" s="42"/>
     </row>
-    <row r="403" spans="1:13">
+    <row r="403" spans="1:13" hidden="1">
       <c r="A403" s="19">
         <v>42975</v>
       </c>
@@ -22193,7 +22197,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="404" spans="1:13">
+    <row r="404" spans="1:13" hidden="1">
       <c r="A404" s="19">
         <v>42975</v>
       </c>
@@ -22221,7 +22225,7 @@
       </c>
       <c r="J404" s="42"/>
     </row>
-    <row r="405" spans="1:13">
+    <row r="405" spans="1:13" hidden="1">
       <c r="A405" s="19">
         <v>42975</v>
       </c>
@@ -22249,7 +22253,7 @@
       </c>
       <c r="J405" s="42"/>
     </row>
-    <row r="406" spans="1:13">
+    <row r="406" spans="1:13" hidden="1">
       <c r="A406" s="19">
         <v>42975</v>
       </c>
@@ -22288,7 +22292,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="407" spans="1:13">
+    <row r="407" spans="1:13" hidden="1">
       <c r="A407" s="19">
         <v>42975</v>
       </c>
@@ -22316,7 +22320,7 @@
       </c>
       <c r="J407" s="42"/>
     </row>
-    <row r="408" spans="1:13">
+    <row r="408" spans="1:13" hidden="1">
       <c r="A408" s="19">
         <v>42975</v>
       </c>
@@ -22344,7 +22348,7 @@
       </c>
       <c r="J408" s="42"/>
     </row>
-    <row r="409" spans="1:13">
+    <row r="409" spans="1:13" hidden="1">
       <c r="A409" s="19">
         <v>42975</v>
       </c>
@@ -22372,7 +22376,7 @@
       </c>
       <c r="J409" s="42"/>
     </row>
-    <row r="410" spans="1:13">
+    <row r="410" spans="1:13" hidden="1">
       <c r="A410" s="19">
         <v>42975</v>
       </c>
@@ -22411,7 +22415,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="411" spans="1:13">
+    <row r="411" spans="1:13" hidden="1">
       <c r="A411" s="19">
         <v>42975</v>
       </c>
@@ -22439,7 +22443,7 @@
       </c>
       <c r="J411" s="42"/>
     </row>
-    <row r="412" spans="1:13">
+    <row r="412" spans="1:13" hidden="1">
       <c r="A412" s="19">
         <v>42975</v>
       </c>
@@ -22478,7 +22482,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="413" spans="1:13">
+    <row r="413" spans="1:13" hidden="1">
       <c r="A413" s="19">
         <v>42975</v>
       </c>
@@ -22506,7 +22510,7 @@
       </c>
       <c r="J413" s="42"/>
     </row>
-    <row r="414" spans="1:13">
+    <row r="414" spans="1:13" hidden="1">
       <c r="A414" s="19">
         <v>42975</v>
       </c>
@@ -22545,7 +22549,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="415" spans="1:13">
+    <row r="415" spans="1:13" hidden="1">
       <c r="A415" s="19">
         <v>42975</v>
       </c>
@@ -22573,7 +22577,7 @@
       </c>
       <c r="J415" s="42"/>
     </row>
-    <row r="416" spans="1:13">
+    <row r="416" spans="1:13" hidden="1">
       <c r="A416" s="19">
         <v>42975</v>
       </c>
@@ -22601,7 +22605,7 @@
       </c>
       <c r="J416" s="42"/>
     </row>
-    <row r="417" spans="1:13">
+    <row r="417" spans="1:13" hidden="1">
       <c r="A417" s="19">
         <v>42975</v>
       </c>
@@ -22629,7 +22633,7 @@
       </c>
       <c r="J417" s="42"/>
     </row>
-    <row r="418" spans="1:13">
+    <row r="418" spans="1:13" hidden="1">
       <c r="A418" s="19">
         <v>42975</v>
       </c>
@@ -22657,7 +22661,7 @@
       </c>
       <c r="J418" s="42"/>
     </row>
-    <row r="419" spans="1:13">
+    <row r="419" spans="1:13" hidden="1">
       <c r="A419" s="19">
         <v>42975</v>
       </c>
@@ -22696,7 +22700,7 @@
         <v>1121</v>
       </c>
     </row>
-    <row r="420" spans="1:13">
+    <row r="420" spans="1:13" hidden="1">
       <c r="A420" s="19">
         <v>42975</v>
       </c>
@@ -22724,7 +22728,7 @@
       </c>
       <c r="J420" s="42"/>
     </row>
-    <row r="421" spans="1:13">
+    <row r="421" spans="1:13" hidden="1">
       <c r="A421" s="19">
         <v>42975</v>
       </c>
@@ -22752,7 +22756,7 @@
       </c>
       <c r="J421" s="42"/>
     </row>
-    <row r="422" spans="1:13">
+    <row r="422" spans="1:13" hidden="1">
       <c r="A422" s="19">
         <v>42975</v>
       </c>
@@ -22780,7 +22784,7 @@
       </c>
       <c r="J422" s="42"/>
     </row>
-    <row r="423" spans="1:13">
+    <row r="423" spans="1:13" hidden="1">
       <c r="A423" s="19">
         <v>42975</v>
       </c>
@@ -22819,7 +22823,7 @@
         <v>1120</v>
       </c>
     </row>
-    <row r="424" spans="1:13">
+    <row r="424" spans="1:13" hidden="1">
       <c r="A424" s="19">
         <v>42975</v>
       </c>
@@ -22847,7 +22851,7 @@
       </c>
       <c r="J424" s="42"/>
     </row>
-    <row r="425" spans="1:13">
+    <row r="425" spans="1:13" hidden="1">
       <c r="A425" s="19">
         <v>42975</v>
       </c>
@@ -22875,7 +22879,7 @@
       </c>
       <c r="J425" s="42"/>
     </row>
-    <row r="426" spans="1:13">
+    <row r="426" spans="1:13" hidden="1">
       <c r="A426" s="19">
         <v>42975</v>
       </c>
@@ -22914,7 +22918,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="427" spans="1:13">
+    <row r="427" spans="1:13" hidden="1">
       <c r="A427" s="19">
         <v>42975</v>
       </c>
@@ -22942,7 +22946,7 @@
       </c>
       <c r="J427" s="42"/>
     </row>
-    <row r="428" spans="1:13">
+    <row r="428" spans="1:13" hidden="1">
       <c r="A428" s="19">
         <v>42975</v>
       </c>
@@ -22970,7 +22974,7 @@
       </c>
       <c r="J428" s="42"/>
     </row>
-    <row r="429" spans="1:13">
+    <row r="429" spans="1:13" hidden="1">
       <c r="A429" s="19">
         <v>42975</v>
       </c>
@@ -22998,7 +23002,7 @@
       </c>
       <c r="J429" s="42"/>
     </row>
-    <row r="430" spans="1:13">
+    <row r="430" spans="1:13" hidden="1">
       <c r="A430" s="19">
         <v>42975</v>
       </c>
@@ -23026,7 +23030,7 @@
       </c>
       <c r="J430" s="42"/>
     </row>
-    <row r="431" spans="1:13">
+    <row r="431" spans="1:13" hidden="1">
       <c r="A431" s="19">
         <v>42975</v>
       </c>
@@ -23054,7 +23058,7 @@
       </c>
       <c r="J431" s="42"/>
     </row>
-    <row r="432" spans="1:13">
+    <row r="432" spans="1:13" hidden="1">
       <c r="A432" s="19">
         <v>42975</v>
       </c>
@@ -23093,7 +23097,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="433" spans="1:13">
+    <row r="433" spans="1:13" hidden="1">
       <c r="A433" s="19">
         <v>42975</v>
       </c>
@@ -23124,7 +23128,7 @@
       </c>
       <c r="J433" s="42"/>
     </row>
-    <row r="434" spans="1:13">
+    <row r="434" spans="1:13" hidden="1">
       <c r="A434" s="19">
         <v>42975</v>
       </c>
@@ -23163,7 +23167,7 @@
         <v>1133</v>
       </c>
     </row>
-    <row r="435" spans="1:13">
+    <row r="435" spans="1:13" hidden="1">
       <c r="A435" s="19">
         <v>42975</v>
       </c>
@@ -23191,7 +23195,7 @@
       </c>
       <c r="J435" s="42"/>
     </row>
-    <row r="436" spans="1:13">
+    <row r="436" spans="1:13" hidden="1">
       <c r="A436" s="19">
         <v>42975</v>
       </c>
@@ -23230,7 +23234,7 @@
         <v>1134</v>
       </c>
     </row>
-    <row r="437" spans="1:13">
+    <row r="437" spans="1:13" hidden="1">
       <c r="A437" s="19">
         <v>42975</v>
       </c>
@@ -23269,7 +23273,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="438" spans="1:13">
+    <row r="438" spans="1:13" hidden="1">
       <c r="A438" s="19">
         <v>42975</v>
       </c>
@@ -23300,7 +23304,7 @@
       </c>
       <c r="J438" s="42"/>
     </row>
-    <row r="439" spans="1:13">
+    <row r="439" spans="1:13" hidden="1">
       <c r="A439" s="19">
         <v>42975</v>
       </c>
@@ -23339,7 +23343,7 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="440" spans="1:13">
+    <row r="440" spans="1:13" hidden="1">
       <c r="A440" s="19">
         <v>42975</v>
       </c>
@@ -23367,7 +23371,7 @@
       </c>
       <c r="J440" s="42"/>
     </row>
-    <row r="441" spans="1:13">
+    <row r="441" spans="1:13" hidden="1">
       <c r="A441" s="19">
         <v>42975</v>
       </c>
@@ -23397,7 +23401,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="442" spans="1:13">
+    <row r="442" spans="1:13" hidden="1">
       <c r="A442" s="19">
         <v>42975</v>
       </c>
@@ -23436,7 +23440,7 @@
         <v>1140</v>
       </c>
     </row>
-    <row r="443" spans="1:13">
+    <row r="443" spans="1:13" hidden="1">
       <c r="A443" s="19">
         <v>42975</v>
       </c>
@@ -23464,7 +23468,7 @@
       </c>
       <c r="J443" s="42"/>
     </row>
-    <row r="444" spans="1:13">
+    <row r="444" spans="1:13" hidden="1">
       <c r="A444" s="19">
         <v>42975</v>
       </c>
@@ -23492,7 +23496,7 @@
       </c>
       <c r="J444" s="42"/>
     </row>
-    <row r="445" spans="1:13">
+    <row r="445" spans="1:13" hidden="1">
       <c r="A445" s="19">
         <v>42975</v>
       </c>
@@ -23528,7 +23532,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="446" spans="1:13">
+    <row r="446" spans="1:13" hidden="1">
       <c r="A446" s="19">
         <v>42975</v>
       </c>
@@ -23564,7 +23568,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="447" spans="1:13">
+    <row r="447" spans="1:13" hidden="1">
       <c r="A447" s="19">
         <v>42975</v>
       </c>
@@ -23612,7 +23616,7 @@
         <v>1105</v>
       </c>
     </row>
-    <row r="449" spans="1:13">
+    <row r="449" spans="1:13" hidden="1">
       <c r="A449" s="19">
         <v>42975</v>
       </c>
@@ -23636,7 +23640,7 @@
         <v>923</v>
       </c>
     </row>
-    <row r="450" spans="1:13">
+    <row r="450" spans="1:13" hidden="1">
       <c r="A450" s="19">
         <v>42975</v>
       </c>
@@ -23660,7 +23664,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="451" spans="1:13">
+    <row r="451" spans="1:13" hidden="1">
       <c r="A451" s="19">
         <v>42975</v>
       </c>
@@ -23696,7 +23700,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="452" spans="1:13">
+    <row r="452" spans="1:13" hidden="1">
       <c r="A452" s="19">
         <v>42975</v>
       </c>
@@ -23723,7 +23727,7 @@
         <v>925</v>
       </c>
     </row>
-    <row r="453" spans="1:13">
+    <row r="453" spans="1:13" hidden="1">
       <c r="A453" s="19">
         <v>42975</v>
       </c>
@@ -23747,7 +23751,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="454" spans="1:13">
+    <row r="454" spans="1:13" hidden="1">
       <c r="A454" s="19">
         <v>42975</v>
       </c>
@@ -23783,7 +23787,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="455" spans="1:13">
+    <row r="455" spans="1:13" hidden="1">
       <c r="A455" s="19">
         <v>42975</v>
       </c>
@@ -23819,7 +23823,7 @@
         <v>1124</v>
       </c>
     </row>
-    <row r="456" spans="1:13">
+    <row r="456" spans="1:13" hidden="1">
       <c r="A456" s="19">
         <v>42975</v>
       </c>
@@ -23843,7 +23847,7 @@
         <v>923</v>
       </c>
     </row>
-    <row r="457" spans="1:13">
+    <row r="457" spans="1:13" hidden="1">
       <c r="A457" s="19">
         <v>42975</v>
       </c>
@@ -23879,7 +23883,7 @@
         <v>1121</v>
       </c>
     </row>
-    <row r="458" spans="1:13">
+    <row r="458" spans="1:13" hidden="1">
       <c r="A458" s="19">
         <v>42975</v>
       </c>
@@ -23915,7 +23919,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="459" spans="1:13">
+    <row r="459" spans="1:13" hidden="1">
       <c r="A459" s="19">
         <v>42975</v>
       </c>
@@ -23939,7 +23943,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="460" spans="1:13">
+    <row r="460" spans="1:13" hidden="1">
       <c r="A460" s="19">
         <v>42975</v>
       </c>
@@ -23963,7 +23967,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="461" spans="1:13">
+    <row r="461" spans="1:13" hidden="1">
       <c r="A461" s="19">
         <v>42975</v>
       </c>
@@ -23999,7 +24003,7 @@
         <v>1135</v>
       </c>
     </row>
-    <row r="462" spans="1:13">
+    <row r="462" spans="1:13" hidden="1">
       <c r="A462" s="19">
         <v>42975</v>
       </c>
@@ -24023,7 +24027,7 @@
         <v>923</v>
       </c>
     </row>
-    <row r="463" spans="1:13">
+    <row r="463" spans="1:13" hidden="1">
       <c r="A463" s="19">
         <v>42975</v>
       </c>
@@ -24050,7 +24054,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="464" spans="1:13">
+    <row r="464" spans="1:13" hidden="1">
       <c r="A464" s="19">
         <v>42975</v>
       </c>
@@ -24086,7 +24090,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="465" spans="1:7">
+    <row r="465" spans="1:7" hidden="1">
       <c r="A465" s="19">
         <v>42975</v>
       </c>
@@ -24102,12 +24106,21 @@
       <c r="F465" s="29">
         <v>12000</v>
       </c>
-      <c r="G465">
+    </row>
+    <row r="466" spans="1:7" hidden="1">
+      <c r="G466">
         <f>SUM(G2:G464)</f>
         <v>9930</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:T466" xr:uid="{7F2C125D-04F2-4AC0-AD38-229DCB16B0E4}">
+    <filterColumn colId="7">
+      <filters>
+        <filter val="P"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>

</xml_diff>